<commit_message>
completed code for single cat
</commit_message>
<xml_diff>
--- a/target/ExcelCalculatorForDistributor/Arshad New Calculator.xlsx
+++ b/target/ExcelCalculatorForDistributor/Arshad New Calculator.xlsx
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13346" uniqueCount="532">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21576" uniqueCount="606">
   <si>
     <t>id</t>
   </si>
@@ -1751,6 +1751,228 @@
   <si>
     <t xml:space="preserve">Basis of Settlement within Network
 </t>
+  </si>
+  <si>
+    <t>18985</t>
+  </si>
+  <si>
+    <t>226</t>
+  </si>
+  <si>
+    <t>2025-01-22 13:51:19</t>
+  </si>
+  <si>
+    <t>18986</t>
+  </si>
+  <si>
+    <t>18987</t>
+  </si>
+  <si>
+    <t>18988</t>
+  </si>
+  <si>
+    <t>18989</t>
+  </si>
+  <si>
+    <t>18990</t>
+  </si>
+  <si>
+    <t>18991</t>
+  </si>
+  <si>
+    <t>18992</t>
+  </si>
+  <si>
+    <t>18993</t>
+  </si>
+  <si>
+    <t>18994</t>
+  </si>
+  <si>
+    <t>18995</t>
+  </si>
+  <si>
+    <t>18996</t>
+  </si>
+  <si>
+    <t>18997</t>
+  </si>
+  <si>
+    <t>18998</t>
+  </si>
+  <si>
+    <t>18999</t>
+  </si>
+  <si>
+    <t>19000</t>
+  </si>
+  <si>
+    <t>19001</t>
+  </si>
+  <si>
+    <t>19002</t>
+  </si>
+  <si>
+    <t>19003</t>
+  </si>
+  <si>
+    <t>19004</t>
+  </si>
+  <si>
+    <t>19005</t>
+  </si>
+  <si>
+    <t>19006</t>
+  </si>
+  <si>
+    <t>19007</t>
+  </si>
+  <si>
+    <t>19008</t>
+  </si>
+  <si>
+    <t>19009</t>
+  </si>
+  <si>
+    <t>19010</t>
+  </si>
+  <si>
+    <t>19011</t>
+  </si>
+  <si>
+    <t>19012</t>
+  </si>
+  <si>
+    <t>19013</t>
+  </si>
+  <si>
+    <t>19014</t>
+  </si>
+  <si>
+    <t>19015</t>
+  </si>
+  <si>
+    <t>19016</t>
+  </si>
+  <si>
+    <t>19017</t>
+  </si>
+  <si>
+    <t>19018</t>
+  </si>
+  <si>
+    <t>19019</t>
+  </si>
+  <si>
+    <t>19020</t>
+  </si>
+  <si>
+    <t>19021</t>
+  </si>
+  <si>
+    <t>19022</t>
+  </si>
+  <si>
+    <t>19023</t>
+  </si>
+  <si>
+    <t>19024</t>
+  </si>
+  <si>
+    <t>19025</t>
+  </si>
+  <si>
+    <t>19026</t>
+  </si>
+  <si>
+    <t>19027</t>
+  </si>
+  <si>
+    <t>19028</t>
+  </si>
+  <si>
+    <t>19029</t>
+  </si>
+  <si>
+    <t>19030</t>
+  </si>
+  <si>
+    <t>19031</t>
+  </si>
+  <si>
+    <t>19032</t>
+  </si>
+  <si>
+    <t>19033</t>
+  </si>
+  <si>
+    <t>19034</t>
+  </si>
+  <si>
+    <t>19035</t>
+  </si>
+  <si>
+    <t>19036</t>
+  </si>
+  <si>
+    <t>19037</t>
+  </si>
+  <si>
+    <t>19038</t>
+  </si>
+  <si>
+    <t>19039</t>
+  </si>
+  <si>
+    <t>19040</t>
+  </si>
+  <si>
+    <t>19041</t>
+  </si>
+  <si>
+    <t>19042</t>
+  </si>
+  <si>
+    <t>19043</t>
+  </si>
+  <si>
+    <t>19044</t>
+  </si>
+  <si>
+    <t>19045</t>
+  </si>
+  <si>
+    <t>19046</t>
+  </si>
+  <si>
+    <t>19047</t>
+  </si>
+  <si>
+    <t>19048</t>
+  </si>
+  <si>
+    <t>19049</t>
+  </si>
+  <si>
+    <t>19050</t>
+  </si>
+  <si>
+    <t>19051</t>
+  </si>
+  <si>
+    <t>19052</t>
+  </si>
+  <si>
+    <t>19053</t>
+  </si>
+  <si>
+    <t>19054</t>
+  </si>
+  <si>
+    <t>19055</t>
+  </si>
+  <si>
+    <t>19056</t>
   </si>
 </sst>
 </file>
@@ -6796,10 +7018,10 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="83" t="s">
-        <v>436</v>
+        <v>532</v>
       </c>
       <c r="B2" s="83" t="s">
-        <v>310</v>
+        <v>533</v>
       </c>
       <c r="C2" s="83" t="s">
         <v>308</v>
@@ -6826,10 +7048,10 @@
         <v>310</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="P2" s="4" t="str">
         <f t="shared" ref="P2:P65" si="0">C2&amp;-D2</f>
@@ -6846,10 +7068,10 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="83" t="s">
-        <v>438</v>
+        <v>535</v>
       </c>
       <c r="B3" s="83" t="s">
-        <v>310</v>
+        <v>533</v>
       </c>
       <c r="C3" s="83" t="s">
         <v>311</v>
@@ -6876,10 +7098,10 @@
         <v>310</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="P3" s="4" t="str">
         <f t="shared" si="0"/>
@@ -6896,10 +7118,10 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="83" t="s">
-        <v>439</v>
+        <v>536</v>
       </c>
       <c r="B4" s="83" t="s">
-        <v>310</v>
+        <v>533</v>
       </c>
       <c r="C4" s="83" t="s">
         <v>313</v>
@@ -6926,10 +7148,10 @@
         <v>310</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="P4" s="4" t="str">
         <f t="shared" si="0"/>
@@ -6946,10 +7168,10 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="83" t="s">
-        <v>440</v>
+        <v>537</v>
       </c>
       <c r="B5" s="83" t="s">
-        <v>310</v>
+        <v>533</v>
       </c>
       <c r="C5" s="83" t="s">
         <v>315</v>
@@ -6976,10 +7198,10 @@
         <v>310</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="P5" s="4" t="str">
         <f t="shared" si="0"/>
@@ -6996,10 +7218,10 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="83" t="s">
-        <v>441</v>
+        <v>538</v>
       </c>
       <c r="B6" s="83" t="s">
-        <v>310</v>
+        <v>533</v>
       </c>
       <c r="C6" s="83" t="s">
         <v>317</v>
@@ -7026,10 +7248,10 @@
         <v>310</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="P6" s="4" t="str">
         <f t="shared" si="0"/>
@@ -7046,10 +7268,10 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="83" t="s">
-        <v>442</v>
+        <v>539</v>
       </c>
       <c r="B7" s="83" t="s">
-        <v>310</v>
+        <v>533</v>
       </c>
       <c r="C7" s="83" t="s">
         <v>319</v>
@@ -7076,10 +7298,10 @@
         <v>310</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="P7" s="4" t="str">
         <f t="shared" si="0"/>
@@ -7096,10 +7318,10 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="83" t="s">
-        <v>443</v>
+        <v>540</v>
       </c>
       <c r="B8" s="83" t="s">
-        <v>310</v>
+        <v>533</v>
       </c>
       <c r="C8" s="83" t="s">
         <v>321</v>
@@ -7126,10 +7348,10 @@
         <v>310</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="P8" s="4" t="str">
         <f t="shared" si="0"/>
@@ -7146,10 +7368,10 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="83" t="s">
-        <v>444</v>
+        <v>541</v>
       </c>
       <c r="B9" s="83" t="s">
-        <v>310</v>
+        <v>533</v>
       </c>
       <c r="C9" s="83" t="s">
         <v>323</v>
@@ -7176,10 +7398,10 @@
         <v>310</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="N9" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="P9" s="4" t="str">
         <f t="shared" si="0"/>
@@ -7196,10 +7418,10 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="83" t="s">
-        <v>445</v>
+        <v>542</v>
       </c>
       <c r="B10" s="83" t="s">
-        <v>310</v>
+        <v>533</v>
       </c>
       <c r="C10" s="83" t="s">
         <v>325</v>
@@ -7226,10 +7448,10 @@
         <v>310</v>
       </c>
       <c r="M10" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="N10" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="P10" s="4" t="str">
         <f t="shared" si="0"/>
@@ -7246,10 +7468,10 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="83" t="s">
-        <v>446</v>
+        <v>543</v>
       </c>
       <c r="B11" s="83" t="s">
-        <v>310</v>
+        <v>533</v>
       </c>
       <c r="C11" s="83" t="s">
         <v>327</v>
@@ -7276,10 +7498,10 @@
         <v>310</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="N11" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="P11" s="4" t="str">
         <f t="shared" si="0"/>
@@ -7296,10 +7518,10 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="83" t="s">
-        <v>447</v>
+        <v>544</v>
       </c>
       <c r="B12" s="83" t="s">
-        <v>310</v>
+        <v>533</v>
       </c>
       <c r="C12" s="83" t="s">
         <v>329</v>
@@ -7326,10 +7548,10 @@
         <v>310</v>
       </c>
       <c r="M12" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="N12" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="P12" s="4" t="str">
         <f t="shared" si="0"/>
@@ -7346,10 +7568,10 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="83" t="s">
-        <v>448</v>
+        <v>545</v>
       </c>
       <c r="B13" s="83" t="s">
-        <v>310</v>
+        <v>533</v>
       </c>
       <c r="C13" s="83" t="s">
         <v>331</v>
@@ -7376,10 +7598,10 @@
         <v>310</v>
       </c>
       <c r="M13" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="N13" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="P13" s="4" t="str">
         <f t="shared" si="0"/>
@@ -7396,10 +7618,10 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="83" t="s">
-        <v>449</v>
+        <v>546</v>
       </c>
       <c r="B14" s="83" t="s">
-        <v>310</v>
+        <v>533</v>
       </c>
       <c r="C14" s="83" t="s">
         <v>308</v>
@@ -7426,10 +7648,10 @@
         <v>310</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="N14" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="P14" s="4" t="str">
         <f t="shared" si="0"/>
@@ -7446,10 +7668,10 @@
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="83" t="s">
-        <v>450</v>
+        <v>547</v>
       </c>
       <c r="B15" s="83" t="s">
-        <v>310</v>
+        <v>533</v>
       </c>
       <c r="C15" s="83" t="s">
         <v>311</v>
@@ -7476,10 +7698,10 @@
         <v>310</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="N15" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="P15" s="4" t="str">
         <f t="shared" si="0"/>
@@ -7496,10 +7718,10 @@
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="83" t="s">
-        <v>451</v>
+        <v>548</v>
       </c>
       <c r="B16" s="83" t="s">
-        <v>310</v>
+        <v>533</v>
       </c>
       <c r="C16" s="83" t="s">
         <v>313</v>
@@ -7526,10 +7748,10 @@
         <v>310</v>
       </c>
       <c r="M16" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="N16" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="P16" s="4" t="str">
         <f t="shared" si="0"/>
@@ -7546,10 +7768,10 @@
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" s="83" t="s">
-        <v>452</v>
+        <v>549</v>
       </c>
       <c r="B17" s="83" t="s">
-        <v>310</v>
+        <v>533</v>
       </c>
       <c r="C17" s="83" t="s">
         <v>315</v>
@@ -7576,10 +7798,10 @@
         <v>310</v>
       </c>
       <c r="M17" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="N17" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="P17" s="4" t="str">
         <f t="shared" si="0"/>
@@ -7596,10 +7818,10 @@
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" s="83" t="s">
-        <v>453</v>
+        <v>550</v>
       </c>
       <c r="B18" s="83" t="s">
-        <v>310</v>
+        <v>533</v>
       </c>
       <c r="C18" s="83" t="s">
         <v>317</v>
@@ -7626,10 +7848,10 @@
         <v>310</v>
       </c>
       <c r="M18" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="N18" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="P18" s="4" t="str">
         <f t="shared" si="0"/>
@@ -7646,10 +7868,10 @@
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" s="83" t="s">
-        <v>454</v>
+        <v>551</v>
       </c>
       <c r="B19" s="83" t="s">
-        <v>310</v>
+        <v>533</v>
       </c>
       <c r="C19" s="83" t="s">
         <v>319</v>
@@ -7676,10 +7898,10 @@
         <v>310</v>
       </c>
       <c r="M19" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="N19" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="P19" s="4" t="str">
         <f t="shared" si="0"/>
@@ -7696,10 +7918,10 @@
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" s="83" t="s">
-        <v>455</v>
+        <v>552</v>
       </c>
       <c r="B20" s="83" t="s">
-        <v>310</v>
+        <v>533</v>
       </c>
       <c r="C20" s="83" t="s">
         <v>321</v>
@@ -7726,10 +7948,10 @@
         <v>310</v>
       </c>
       <c r="M20" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="N20" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="P20" s="4" t="str">
         <f t="shared" si="0"/>
@@ -7746,10 +7968,10 @@
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21" s="83" t="s">
-        <v>456</v>
+        <v>553</v>
       </c>
       <c r="B21" s="83" t="s">
-        <v>310</v>
+        <v>533</v>
       </c>
       <c r="C21" s="83" t="s">
         <v>323</v>
@@ -7776,10 +7998,10 @@
         <v>310</v>
       </c>
       <c r="M21" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="N21" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="P21" s="4" t="str">
         <f t="shared" si="0"/>
@@ -7796,10 +8018,10 @@
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22" s="83" t="s">
-        <v>457</v>
+        <v>554</v>
       </c>
       <c r="B22" s="83" t="s">
-        <v>310</v>
+        <v>533</v>
       </c>
       <c r="C22" s="83" t="s">
         <v>325</v>
@@ -7826,10 +8048,10 @@
         <v>310</v>
       </c>
       <c r="M22" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="N22" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="P22" s="4" t="str">
         <f t="shared" si="0"/>
@@ -7846,10 +8068,10 @@
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" s="83" t="s">
-        <v>458</v>
+        <v>555</v>
       </c>
       <c r="B23" s="83" t="s">
-        <v>310</v>
+        <v>533</v>
       </c>
       <c r="C23" s="83" t="s">
         <v>327</v>
@@ -7876,10 +8098,10 @@
         <v>310</v>
       </c>
       <c r="M23" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="N23" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="P23" s="4" t="str">
         <f t="shared" si="0"/>
@@ -7896,10 +8118,10 @@
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24" s="83" t="s">
-        <v>459</v>
+        <v>556</v>
       </c>
       <c r="B24" s="83" t="s">
-        <v>310</v>
+        <v>533</v>
       </c>
       <c r="C24" s="83" t="s">
         <v>329</v>
@@ -7926,10 +8148,10 @@
         <v>310</v>
       </c>
       <c r="M24" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="N24" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="P24" s="4" t="str">
         <f t="shared" si="0"/>
@@ -7946,10 +8168,10 @@
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25" s="83" t="s">
-        <v>460</v>
+        <v>557</v>
       </c>
       <c r="B25" s="83" t="s">
-        <v>310</v>
+        <v>533</v>
       </c>
       <c r="C25" s="83" t="s">
         <v>331</v>
@@ -7976,10 +8198,10 @@
         <v>310</v>
       </c>
       <c r="M25" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="N25" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="P25" s="4" t="str">
         <f t="shared" si="0"/>
@@ -7996,10 +8218,10 @@
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A26" s="83" t="s">
-        <v>461</v>
+        <v>558</v>
       </c>
       <c r="B26" s="83" t="s">
-        <v>310</v>
+        <v>533</v>
       </c>
       <c r="C26" s="83" t="s">
         <v>308</v>
@@ -8026,10 +8248,10 @@
         <v>310</v>
       </c>
       <c r="M26" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="N26" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="P26" s="4" t="str">
         <f t="shared" si="0"/>
@@ -8046,10 +8268,10 @@
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A27" s="83" t="s">
-        <v>462</v>
+        <v>559</v>
       </c>
       <c r="B27" s="83" t="s">
-        <v>310</v>
+        <v>533</v>
       </c>
       <c r="C27" s="83" t="s">
         <v>311</v>
@@ -8076,10 +8298,10 @@
         <v>310</v>
       </c>
       <c r="M27" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="N27" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="P27" s="4" t="str">
         <f t="shared" si="0"/>
@@ -8096,10 +8318,10 @@
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28" s="83" t="s">
-        <v>463</v>
+        <v>560</v>
       </c>
       <c r="B28" s="83" t="s">
-        <v>310</v>
+        <v>533</v>
       </c>
       <c r="C28" s="83" t="s">
         <v>313</v>
@@ -8128,10 +8350,10 @@
         <v>310</v>
       </c>
       <c r="M28" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="N28" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="P28" s="4" t="str">
         <f t="shared" si="0"/>
@@ -8148,10 +8370,10 @@
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A29" s="83" t="s">
-        <v>464</v>
+        <v>561</v>
       </c>
       <c r="B29" s="83" t="s">
-        <v>310</v>
+        <v>533</v>
       </c>
       <c r="C29" s="83" t="s">
         <v>315</v>
@@ -8180,10 +8402,10 @@
         <v>310</v>
       </c>
       <c r="M29" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="N29" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="P29" s="4" t="str">
         <f t="shared" si="0"/>
@@ -8200,10 +8422,10 @@
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A30" s="83" t="s">
-        <v>465</v>
+        <v>562</v>
       </c>
       <c r="B30" s="83" t="s">
-        <v>310</v>
+        <v>533</v>
       </c>
       <c r="C30" s="83" t="s">
         <v>317</v>
@@ -8232,10 +8454,10 @@
         <v>310</v>
       </c>
       <c r="M30" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="N30" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="P30" s="4" t="str">
         <f t="shared" si="0"/>
@@ -8252,10 +8474,10 @@
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A31" s="83" t="s">
-        <v>466</v>
+        <v>563</v>
       </c>
       <c r="B31" s="83" t="s">
-        <v>310</v>
+        <v>533</v>
       </c>
       <c r="C31" s="83" t="s">
         <v>319</v>
@@ -8284,10 +8506,10 @@
         <v>310</v>
       </c>
       <c r="M31" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="N31" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="P31" s="4" t="str">
         <f t="shared" si="0"/>
@@ -8304,10 +8526,10 @@
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A32" s="83" t="s">
-        <v>467</v>
+        <v>564</v>
       </c>
       <c r="B32" s="83" t="s">
-        <v>310</v>
+        <v>533</v>
       </c>
       <c r="C32" s="83" t="s">
         <v>321</v>
@@ -8336,10 +8558,10 @@
         <v>310</v>
       </c>
       <c r="M32" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="N32" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="P32" s="4" t="str">
         <f t="shared" si="0"/>
@@ -8356,10 +8578,10 @@
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A33" s="83" t="s">
-        <v>468</v>
+        <v>565</v>
       </c>
       <c r="B33" s="83" t="s">
-        <v>310</v>
+        <v>533</v>
       </c>
       <c r="C33" s="83" t="s">
         <v>323</v>
@@ -8386,10 +8608,10 @@
         <v>310</v>
       </c>
       <c r="M33" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="N33" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="P33" s="4" t="str">
         <f t="shared" si="0"/>
@@ -8406,10 +8628,10 @@
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A34" s="83" t="s">
-        <v>469</v>
+        <v>566</v>
       </c>
       <c r="B34" s="83" t="s">
-        <v>310</v>
+        <v>533</v>
       </c>
       <c r="C34" s="83" t="s">
         <v>325</v>
@@ -8436,10 +8658,10 @@
         <v>310</v>
       </c>
       <c r="M34" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="N34" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="P34" s="4" t="str">
         <f t="shared" si="0"/>
@@ -8456,10 +8678,10 @@
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A35" s="83" t="s">
-        <v>470</v>
+        <v>567</v>
       </c>
       <c r="B35" s="83" t="s">
-        <v>310</v>
+        <v>533</v>
       </c>
       <c r="C35" s="83" t="s">
         <v>327</v>
@@ -8486,10 +8708,10 @@
         <v>310</v>
       </c>
       <c r="M35" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="N35" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="P35" s="4" t="str">
         <f t="shared" si="0"/>
@@ -8506,10 +8728,10 @@
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A36" s="83" t="s">
-        <v>471</v>
+        <v>568</v>
       </c>
       <c r="B36" s="83" t="s">
-        <v>310</v>
+        <v>533</v>
       </c>
       <c r="C36" s="83" t="s">
         <v>329</v>
@@ -8536,10 +8758,10 @@
         <v>310</v>
       </c>
       <c r="M36" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="N36" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="P36" s="4" t="str">
         <f t="shared" si="0"/>
@@ -8556,10 +8778,10 @@
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A37" s="83" t="s">
-        <v>472</v>
+        <v>569</v>
       </c>
       <c r="B37" s="83" t="s">
-        <v>310</v>
+        <v>533</v>
       </c>
       <c r="C37" s="83" t="s">
         <v>331</v>
@@ -8586,10 +8808,10 @@
         <v>310</v>
       </c>
       <c r="M37" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="N37" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="P37" s="4" t="str">
         <f t="shared" si="0"/>
@@ -8606,10 +8828,10 @@
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A38" s="83" t="s">
-        <v>473</v>
+        <v>570</v>
       </c>
       <c r="B38" s="83" t="s">
-        <v>310</v>
+        <v>533</v>
       </c>
       <c r="C38" s="83" t="s">
         <v>308</v>
@@ -8636,10 +8858,10 @@
         <v>310</v>
       </c>
       <c r="M38" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="N38" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="P38" s="4" t="str">
         <f t="shared" si="0"/>
@@ -8656,10 +8878,10 @@
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A39" s="83" t="s">
-        <v>474</v>
+        <v>571</v>
       </c>
       <c r="B39" s="83" t="s">
-        <v>310</v>
+        <v>533</v>
       </c>
       <c r="C39" s="83" t="s">
         <v>311</v>
@@ -8686,10 +8908,10 @@
         <v>310</v>
       </c>
       <c r="M39" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="N39" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="P39" s="4" t="str">
         <f t="shared" si="0"/>
@@ -8706,10 +8928,10 @@
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A40" s="83" t="s">
-        <v>475</v>
+        <v>572</v>
       </c>
       <c r="B40" s="83" t="s">
-        <v>310</v>
+        <v>533</v>
       </c>
       <c r="C40" s="83" t="s">
         <v>313</v>
@@ -8736,10 +8958,10 @@
         <v>310</v>
       </c>
       <c r="M40" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="N40" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="P40" s="4" t="str">
         <f t="shared" si="0"/>
@@ -8756,10 +8978,10 @@
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A41" s="83" t="s">
-        <v>476</v>
+        <v>573</v>
       </c>
       <c r="B41" s="83" t="s">
-        <v>310</v>
+        <v>533</v>
       </c>
       <c r="C41" s="83" t="s">
         <v>315</v>
@@ -8786,10 +9008,10 @@
         <v>310</v>
       </c>
       <c r="M41" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="N41" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="P41" s="4" t="str">
         <f t="shared" si="0"/>
@@ -8806,10 +9028,10 @@
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A42" s="83" t="s">
-        <v>477</v>
+        <v>574</v>
       </c>
       <c r="B42" s="83" t="s">
-        <v>310</v>
+        <v>533</v>
       </c>
       <c r="C42" s="83" t="s">
         <v>317</v>
@@ -8836,10 +9058,10 @@
         <v>310</v>
       </c>
       <c r="M42" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="N42" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="P42" s="4" t="str">
         <f t="shared" si="0"/>
@@ -8856,10 +9078,10 @@
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A43" s="83" t="s">
-        <v>478</v>
+        <v>575</v>
       </c>
       <c r="B43" s="83" t="s">
-        <v>310</v>
+        <v>533</v>
       </c>
       <c r="C43" s="83" t="s">
         <v>319</v>
@@ -8886,10 +9108,10 @@
         <v>310</v>
       </c>
       <c r="M43" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="N43" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="P43" s="4" t="str">
         <f t="shared" si="0"/>
@@ -8906,10 +9128,10 @@
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A44" s="83" t="s">
-        <v>479</v>
+        <v>576</v>
       </c>
       <c r="B44" s="83" t="s">
-        <v>310</v>
+        <v>533</v>
       </c>
       <c r="C44" s="83" t="s">
         <v>321</v>
@@ -8936,10 +9158,10 @@
         <v>310</v>
       </c>
       <c r="M44" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="N44" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="P44" s="4" t="str">
         <f t="shared" si="0"/>
@@ -8956,10 +9178,10 @@
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A45" s="83" t="s">
-        <v>480</v>
+        <v>577</v>
       </c>
       <c r="B45" s="83" t="s">
-        <v>310</v>
+        <v>533</v>
       </c>
       <c r="C45" s="83" t="s">
         <v>323</v>
@@ -8986,10 +9208,10 @@
         <v>310</v>
       </c>
       <c r="M45" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="N45" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="P45" s="4" t="str">
         <f t="shared" si="0"/>
@@ -9006,10 +9228,10 @@
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A46" s="83" t="s">
-        <v>481</v>
+        <v>578</v>
       </c>
       <c r="B46" s="83" t="s">
-        <v>310</v>
+        <v>533</v>
       </c>
       <c r="C46" s="83" t="s">
         <v>325</v>
@@ -9036,10 +9258,10 @@
         <v>310</v>
       </c>
       <c r="M46" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="N46" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="P46" s="4" t="str">
         <f t="shared" si="0"/>
@@ -9056,10 +9278,10 @@
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A47" s="83" t="s">
-        <v>482</v>
+        <v>579</v>
       </c>
       <c r="B47" s="83" t="s">
-        <v>310</v>
+        <v>533</v>
       </c>
       <c r="C47" s="83" t="s">
         <v>327</v>
@@ -9086,10 +9308,10 @@
         <v>310</v>
       </c>
       <c r="M47" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="N47" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="P47" s="4" t="str">
         <f t="shared" si="0"/>
@@ -9106,10 +9328,10 @@
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A48" s="83" t="s">
-        <v>483</v>
+        <v>580</v>
       </c>
       <c r="B48" s="83" t="s">
-        <v>310</v>
+        <v>533</v>
       </c>
       <c r="C48" s="83" t="s">
         <v>329</v>
@@ -9136,10 +9358,10 @@
         <v>310</v>
       </c>
       <c r="M48" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="N48" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="P48" s="4" t="str">
         <f t="shared" si="0"/>
@@ -9156,10 +9378,10 @@
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A49" s="83" t="s">
-        <v>484</v>
+        <v>581</v>
       </c>
       <c r="B49" s="83" t="s">
-        <v>310</v>
+        <v>533</v>
       </c>
       <c r="C49" s="83" t="s">
         <v>331</v>
@@ -9186,10 +9408,10 @@
         <v>310</v>
       </c>
       <c r="M49" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="N49" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="P49" s="4" t="str">
         <f t="shared" si="0"/>
@@ -9206,10 +9428,10 @@
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A50" s="83" t="s">
-        <v>485</v>
+        <v>582</v>
       </c>
       <c r="B50" s="83" t="s">
-        <v>310</v>
+        <v>533</v>
       </c>
       <c r="C50" s="83" t="s">
         <v>308</v>
@@ -9236,10 +9458,10 @@
         <v>310</v>
       </c>
       <c r="M50" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="N50" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="P50" s="4" t="str">
         <f t="shared" si="0"/>
@@ -9256,10 +9478,10 @@
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A51" s="83" t="s">
-        <v>486</v>
+        <v>583</v>
       </c>
       <c r="B51" s="83" t="s">
-        <v>310</v>
+        <v>533</v>
       </c>
       <c r="C51" s="83" t="s">
         <v>311</v>
@@ -9286,10 +9508,10 @@
         <v>310</v>
       </c>
       <c r="M51" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="N51" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="P51" s="4" t="str">
         <f t="shared" si="0"/>
@@ -9306,10 +9528,10 @@
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A52" s="83" t="s">
-        <v>487</v>
+        <v>584</v>
       </c>
       <c r="B52" s="83" t="s">
-        <v>310</v>
+        <v>533</v>
       </c>
       <c r="C52" s="83" t="s">
         <v>313</v>
@@ -9336,10 +9558,10 @@
         <v>310</v>
       </c>
       <c r="M52" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="N52" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="P52" s="4" t="str">
         <f t="shared" si="0"/>
@@ -9356,10 +9578,10 @@
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A53" s="83" t="s">
-        <v>488</v>
+        <v>585</v>
       </c>
       <c r="B53" s="83" t="s">
-        <v>310</v>
+        <v>533</v>
       </c>
       <c r="C53" s="83" t="s">
         <v>315</v>
@@ -9386,10 +9608,10 @@
         <v>310</v>
       </c>
       <c r="M53" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="N53" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="P53" s="4" t="str">
         <f t="shared" si="0"/>
@@ -9406,10 +9628,10 @@
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A54" s="83" t="s">
-        <v>489</v>
+        <v>586</v>
       </c>
       <c r="B54" s="83" t="s">
-        <v>310</v>
+        <v>533</v>
       </c>
       <c r="C54" s="83" t="s">
         <v>317</v>
@@ -9436,10 +9658,10 @@
         <v>310</v>
       </c>
       <c r="M54" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="N54" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="P54" s="4" t="str">
         <f t="shared" si="0"/>
@@ -9456,10 +9678,10 @@
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A55" s="83" t="s">
-        <v>490</v>
+        <v>587</v>
       </c>
       <c r="B55" s="83" t="s">
-        <v>310</v>
+        <v>533</v>
       </c>
       <c r="C55" s="83" t="s">
         <v>319</v>
@@ -9486,10 +9708,10 @@
         <v>310</v>
       </c>
       <c r="M55" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="N55" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="P55" s="4" t="str">
         <f t="shared" si="0"/>
@@ -9506,10 +9728,10 @@
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A56" s="83" t="s">
-        <v>491</v>
+        <v>588</v>
       </c>
       <c r="B56" s="83" t="s">
-        <v>310</v>
+        <v>533</v>
       </c>
       <c r="C56" s="83" t="s">
         <v>321</v>
@@ -9536,10 +9758,10 @@
         <v>310</v>
       </c>
       <c r="M56" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="N56" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="P56" s="4" t="str">
         <f t="shared" si="0"/>
@@ -9556,10 +9778,10 @@
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A57" s="83" t="s">
-        <v>492</v>
+        <v>589</v>
       </c>
       <c r="B57" s="83" t="s">
-        <v>310</v>
+        <v>533</v>
       </c>
       <c r="C57" s="83" t="s">
         <v>323</v>
@@ -9586,10 +9808,10 @@
         <v>310</v>
       </c>
       <c r="M57" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="N57" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="P57" s="4" t="str">
         <f t="shared" si="0"/>
@@ -9606,10 +9828,10 @@
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A58" s="83" t="s">
-        <v>493</v>
+        <v>590</v>
       </c>
       <c r="B58" s="83" t="s">
-        <v>310</v>
+        <v>533</v>
       </c>
       <c r="C58" s="83" t="s">
         <v>325</v>
@@ -9636,10 +9858,10 @@
         <v>310</v>
       </c>
       <c r="M58" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="N58" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="P58" s="4" t="str">
         <f t="shared" si="0"/>
@@ -9656,10 +9878,10 @@
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A59" s="83" t="s">
-        <v>494</v>
+        <v>591</v>
       </c>
       <c r="B59" s="83" t="s">
-        <v>310</v>
+        <v>533</v>
       </c>
       <c r="C59" s="83" t="s">
         <v>327</v>
@@ -9686,10 +9908,10 @@
         <v>310</v>
       </c>
       <c r="M59" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="N59" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="P59" s="4" t="str">
         <f t="shared" si="0"/>
@@ -9706,10 +9928,10 @@
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A60" s="83" t="s">
-        <v>495</v>
+        <v>592</v>
       </c>
       <c r="B60" s="83" t="s">
-        <v>310</v>
+        <v>533</v>
       </c>
       <c r="C60" s="83" t="s">
         <v>329</v>
@@ -9736,10 +9958,10 @@
         <v>310</v>
       </c>
       <c r="M60" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="N60" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="P60" s="4" t="str">
         <f t="shared" si="0"/>
@@ -9756,10 +9978,10 @@
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A61" s="83" t="s">
-        <v>496</v>
+        <v>593</v>
       </c>
       <c r="B61" s="83" t="s">
-        <v>310</v>
+        <v>533</v>
       </c>
       <c r="C61" s="83" t="s">
         <v>331</v>
@@ -9786,10 +10008,10 @@
         <v>310</v>
       </c>
       <c r="M61" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="N61" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="P61" s="4" t="str">
         <f t="shared" si="0"/>
@@ -9806,10 +10028,10 @@
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A62" s="83" t="s">
-        <v>497</v>
+        <v>594</v>
       </c>
       <c r="B62" s="83" t="s">
-        <v>310</v>
+        <v>533</v>
       </c>
       <c r="C62" s="83" t="s">
         <v>308</v>
@@ -9836,10 +10058,10 @@
         <v>310</v>
       </c>
       <c r="M62" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="N62" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="P62" s="4" t="str">
         <f t="shared" si="0"/>
@@ -9856,10 +10078,10 @@
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A63" s="83" t="s">
-        <v>498</v>
+        <v>595</v>
       </c>
       <c r="B63" s="83" t="s">
-        <v>310</v>
+        <v>533</v>
       </c>
       <c r="C63" s="83" t="s">
         <v>311</v>
@@ -9886,10 +10108,10 @@
         <v>310</v>
       </c>
       <c r="M63" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="N63" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="P63" s="4" t="str">
         <f t="shared" si="0"/>
@@ -9906,10 +10128,10 @@
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A64" s="83" t="s">
-        <v>499</v>
+        <v>596</v>
       </c>
       <c r="B64" s="83" t="s">
-        <v>310</v>
+        <v>533</v>
       </c>
       <c r="C64" s="83" t="s">
         <v>313</v>
@@ -9938,10 +10160,10 @@
         <v>310</v>
       </c>
       <c r="M64" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="N64" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="P64" s="4" t="str">
         <f t="shared" si="0"/>
@@ -9958,10 +10180,10 @@
     </row>
     <row r="65" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A65" s="83" t="s">
-        <v>500</v>
+        <v>597</v>
       </c>
       <c r="B65" s="83" t="s">
-        <v>310</v>
+        <v>533</v>
       </c>
       <c r="C65" s="83" t="s">
         <v>315</v>
@@ -9990,10 +10212,10 @@
         <v>310</v>
       </c>
       <c r="M65" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="N65" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="P65" s="4" t="str">
         <f t="shared" si="0"/>
@@ -10010,10 +10232,10 @@
     </row>
     <row r="66" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A66" s="83" t="s">
-        <v>501</v>
+        <v>598</v>
       </c>
       <c r="B66" s="83" t="s">
-        <v>310</v>
+        <v>533</v>
       </c>
       <c r="C66" s="83" t="s">
         <v>317</v>
@@ -10042,10 +10264,10 @@
         <v>310</v>
       </c>
       <c r="M66" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="N66" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="P66" s="4" t="str">
         <f t="shared" ref="P66:P129" si="3">C66&amp;-D66</f>
@@ -10062,10 +10284,10 @@
     </row>
     <row r="67" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A67" s="83" t="s">
-        <v>502</v>
+        <v>599</v>
       </c>
       <c r="B67" s="83" t="s">
-        <v>310</v>
+        <v>533</v>
       </c>
       <c r="C67" s="83" t="s">
         <v>319</v>
@@ -10094,10 +10316,10 @@
         <v>310</v>
       </c>
       <c r="M67" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="N67" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="P67" s="4" t="str">
         <f t="shared" si="3"/>
@@ -10114,10 +10336,10 @@
     </row>
     <row r="68" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A68" s="83" t="s">
-        <v>503</v>
+        <v>600</v>
       </c>
       <c r="B68" s="83" t="s">
-        <v>310</v>
+        <v>533</v>
       </c>
       <c r="C68" s="83" t="s">
         <v>321</v>
@@ -10146,10 +10368,10 @@
         <v>310</v>
       </c>
       <c r="M68" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="N68" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="P68" s="4" t="str">
         <f t="shared" si="3"/>
@@ -10166,10 +10388,10 @@
     </row>
     <row r="69" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A69" s="83" t="s">
-        <v>504</v>
+        <v>601</v>
       </c>
       <c r="B69" s="83" t="s">
-        <v>310</v>
+        <v>533</v>
       </c>
       <c r="C69" s="83" t="s">
         <v>323</v>
@@ -10196,10 +10418,10 @@
         <v>310</v>
       </c>
       <c r="M69" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="N69" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="P69" s="4" t="str">
         <f t="shared" si="3"/>
@@ -10216,10 +10438,10 @@
     </row>
     <row r="70" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A70" s="83" t="s">
-        <v>505</v>
+        <v>602</v>
       </c>
       <c r="B70" s="83" t="s">
-        <v>310</v>
+        <v>533</v>
       </c>
       <c r="C70" s="83" t="s">
         <v>325</v>
@@ -10246,10 +10468,10 @@
         <v>310</v>
       </c>
       <c r="M70" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="N70" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="P70" s="4" t="str">
         <f t="shared" si="3"/>
@@ -10266,10 +10488,10 @@
     </row>
     <row r="71" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A71" s="83" t="s">
-        <v>506</v>
+        <v>603</v>
       </c>
       <c r="B71" s="83" t="s">
-        <v>310</v>
+        <v>533</v>
       </c>
       <c r="C71" s="83" t="s">
         <v>327</v>
@@ -10296,10 +10518,10 @@
         <v>310</v>
       </c>
       <c r="M71" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="N71" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="P71" s="4" t="str">
         <f t="shared" si="3"/>
@@ -10316,10 +10538,10 @@
     </row>
     <row r="72" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A72" s="83" t="s">
-        <v>507</v>
+        <v>604</v>
       </c>
       <c r="B72" s="83" t="s">
-        <v>310</v>
+        <v>533</v>
       </c>
       <c r="C72" s="83" t="s">
         <v>329</v>
@@ -10346,10 +10568,10 @@
         <v>310</v>
       </c>
       <c r="M72" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="N72" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="P72" s="4" t="str">
         <f t="shared" si="3"/>
@@ -10366,10 +10588,10 @@
     </row>
     <row r="73" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A73" s="83" t="s">
-        <v>508</v>
+        <v>605</v>
       </c>
       <c r="B73" s="83" t="s">
-        <v>310</v>
+        <v>533</v>
       </c>
       <c r="C73" s="83" t="s">
         <v>331</v>
@@ -10396,10 +10618,10 @@
         <v>310</v>
       </c>
       <c r="M73" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="N73" s="4" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="P73" s="4" t="str">
         <f t="shared" si="3"/>
@@ -52649,7 +52871,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{937BFF78-0E8F-43A8-8402-97D478674A28}">
-  <dimension ref="A1:P25"/>
+  <dimension ref="A1:P31"/>
   <sheetViews>
     <sheetView zoomScale="109" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
@@ -52892,6 +53114,54 @@
         <v>246</v>
       </c>
     </row>
+    <row r="26">
+      <c r="A26" t="s" s="1">
+        <v>252</v>
+      </c>
+      <c r="B26" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s" s="1">
+        <v>253</v>
+      </c>
+      <c r="B27" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s" s="1">
+        <v>254</v>
+      </c>
+      <c r="B28" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s" s="1">
+        <v>255</v>
+      </c>
+      <c r="B29" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s" s="1">
+        <v>256</v>
+      </c>
+      <c r="B30" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s" s="1">
+        <v>257</v>
+      </c>
+      <c r="B31" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -52902,7 +53172,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94A9421B-ED15-4F79-A02C-835BE7F65A62}">
-  <dimension ref="A1:P11"/>
+  <dimension ref="A1:P51"/>
   <sheetViews>
     <sheetView zoomScale="109" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -52957,7 +53227,7 @@
         <v>258</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>259</v>
+        <v>246</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
@@ -52968,7 +53238,7 @@
         <v>260</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>261</v>
+        <v>246</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
@@ -52979,7 +53249,7 @@
         <v>262</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>261</v>
+        <v>246</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
@@ -52990,7 +53260,7 @@
         <v>263</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>261</v>
+        <v>246</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
@@ -53001,7 +53271,7 @@
         <v>264</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>261</v>
+        <v>246</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
@@ -53012,7 +53282,7 @@
         <v>265</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>261</v>
+        <v>246</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
@@ -53023,7 +53293,7 @@
         <v>266</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>261</v>
+        <v>246</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
@@ -53034,7 +53304,7 @@
         <v>267</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>268</v>
+        <v>246</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
@@ -53045,7 +53315,7 @@
         <v>269</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>268</v>
+        <v>246</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
@@ -53056,7 +53326,447 @@
         <v>270</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>268</v>
+        <v>246</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="1">
+        <v>179</v>
+      </c>
+      <c r="B12" t="s" s="1">
+        <v>258</v>
+      </c>
+      <c r="C12" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B13" t="s" s="1">
+        <v>260</v>
+      </c>
+      <c r="C13" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B14" t="s" s="1">
+        <v>262</v>
+      </c>
+      <c r="C14" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B15" t="s" s="1">
+        <v>263</v>
+      </c>
+      <c r="C15" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B16" t="s" s="1">
+        <v>264</v>
+      </c>
+      <c r="C16" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B17" t="s" s="1">
+        <v>265</v>
+      </c>
+      <c r="C17" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B18" t="s" s="1">
+        <v>266</v>
+      </c>
+      <c r="C18" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s" s="1">
+        <v>190</v>
+      </c>
+      <c r="B19" t="s" s="1">
+        <v>267</v>
+      </c>
+      <c r="C19" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s" s="1">
+        <v>190</v>
+      </c>
+      <c r="B20" t="s" s="1">
+        <v>269</v>
+      </c>
+      <c r="C20" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s" s="1">
+        <v>190</v>
+      </c>
+      <c r="B21" t="s" s="1">
+        <v>270</v>
+      </c>
+      <c r="C21" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s" s="1">
+        <v>179</v>
+      </c>
+      <c r="B22" t="s" s="1">
+        <v>258</v>
+      </c>
+      <c r="C22" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B23" t="s" s="1">
+        <v>260</v>
+      </c>
+      <c r="C23" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B24" t="s" s="1">
+        <v>262</v>
+      </c>
+      <c r="C24" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B25" t="s" s="1">
+        <v>263</v>
+      </c>
+      <c r="C25" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B26" t="s" s="1">
+        <v>264</v>
+      </c>
+      <c r="C26" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B27" t="s" s="1">
+        <v>265</v>
+      </c>
+      <c r="C27" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B28" t="s" s="1">
+        <v>266</v>
+      </c>
+      <c r="C28" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s" s="1">
+        <v>190</v>
+      </c>
+      <c r="B29" t="s" s="1">
+        <v>267</v>
+      </c>
+      <c r="C29" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s" s="1">
+        <v>190</v>
+      </c>
+      <c r="B30" t="s" s="1">
+        <v>269</v>
+      </c>
+      <c r="C30" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s" s="1">
+        <v>190</v>
+      </c>
+      <c r="B31" t="s" s="1">
+        <v>270</v>
+      </c>
+      <c r="C31" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s" s="1">
+        <v>179</v>
+      </c>
+      <c r="B32" t="s" s="1">
+        <v>258</v>
+      </c>
+      <c r="C32" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B33" t="s" s="1">
+        <v>260</v>
+      </c>
+      <c r="C33" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B34" t="s" s="1">
+        <v>262</v>
+      </c>
+      <c r="C34" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B35" t="s" s="1">
+        <v>263</v>
+      </c>
+      <c r="C35" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B36" t="s" s="1">
+        <v>264</v>
+      </c>
+      <c r="C36" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B37" t="s" s="1">
+        <v>265</v>
+      </c>
+      <c r="C37" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B38" t="s" s="1">
+        <v>266</v>
+      </c>
+      <c r="C38" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s" s="1">
+        <v>190</v>
+      </c>
+      <c r="B39" t="s" s="1">
+        <v>267</v>
+      </c>
+      <c r="C39" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s" s="1">
+        <v>190</v>
+      </c>
+      <c r="B40" t="s" s="1">
+        <v>269</v>
+      </c>
+      <c r="C40" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s" s="1">
+        <v>190</v>
+      </c>
+      <c r="B41" t="s" s="1">
+        <v>270</v>
+      </c>
+      <c r="C41" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s" s="1">
+        <v>179</v>
+      </c>
+      <c r="B42" t="s" s="1">
+        <v>258</v>
+      </c>
+      <c r="C42" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B43" t="s" s="1">
+        <v>260</v>
+      </c>
+      <c r="C43" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B44" t="s" s="1">
+        <v>262</v>
+      </c>
+      <c r="C44" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B45" t="s" s="1">
+        <v>263</v>
+      </c>
+      <c r="C45" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B46" t="s" s="1">
+        <v>264</v>
+      </c>
+      <c r="C46" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B47" t="s" s="1">
+        <v>265</v>
+      </c>
+      <c r="C47" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B48" t="s" s="1">
+        <v>266</v>
+      </c>
+      <c r="C48" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s" s="1">
+        <v>190</v>
+      </c>
+      <c r="B49" t="s" s="1">
+        <v>267</v>
+      </c>
+      <c r="C49" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s" s="1">
+        <v>190</v>
+      </c>
+      <c r="B50" t="s" s="1">
+        <v>269</v>
+      </c>
+      <c r="C50" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s" s="1">
+        <v>190</v>
+      </c>
+      <c r="B51" t="s" s="1">
+        <v>270</v>
+      </c>
+      <c r="C51" t="s" s="1">
+        <v>246</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed code foe single cat
</commit_message>
<xml_diff>
--- a/target/ExcelCalculatorForDistributor/Arshad New Calculator.xlsx
+++ b/target/ExcelCalculatorForDistributor/Arshad New Calculator.xlsx
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21576" uniqueCount="606">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42443" uniqueCount="865">
   <si>
     <t>id</t>
   </si>
@@ -1973,6 +1973,794 @@
   </si>
   <si>
     <t>19056</t>
+  </si>
+  <si>
+    <t>51645</t>
+  </si>
+  <si>
+    <t>19557</t>
+  </si>
+  <si>
+    <t>37612</t>
+  </si>
+  <si>
+    <t>1601</t>
+  </si>
+  <si>
+    <t>TEST-ABC-0125-1-00052</t>
+  </si>
+  <si>
+    <t>51646</t>
+  </si>
+  <si>
+    <t>19558</t>
+  </si>
+  <si>
+    <t>37616</t>
+  </si>
+  <si>
+    <t>51647</t>
+  </si>
+  <si>
+    <t>19559</t>
+  </si>
+  <si>
+    <t>37617</t>
+  </si>
+  <si>
+    <t>51648</t>
+  </si>
+  <si>
+    <t>19560</t>
+  </si>
+  <si>
+    <t>37621</t>
+  </si>
+  <si>
+    <t>51649</t>
+  </si>
+  <si>
+    <t>19561</t>
+  </si>
+  <si>
+    <t>37622</t>
+  </si>
+  <si>
+    <t>51650</t>
+  </si>
+  <si>
+    <t>19562</t>
+  </si>
+  <si>
+    <t>37623</t>
+  </si>
+  <si>
+    <t>51651</t>
+  </si>
+  <si>
+    <t>19563</t>
+  </si>
+  <si>
+    <t>37624</t>
+  </si>
+  <si>
+    <t>51652</t>
+  </si>
+  <si>
+    <t>19564</t>
+  </si>
+  <si>
+    <t>37625</t>
+  </si>
+  <si>
+    <t>51653</t>
+  </si>
+  <si>
+    <t>19565</t>
+  </si>
+  <si>
+    <t>37626</t>
+  </si>
+  <si>
+    <t>51654</t>
+  </si>
+  <si>
+    <t>19566</t>
+  </si>
+  <si>
+    <t>37627</t>
+  </si>
+  <si>
+    <t>51655</t>
+  </si>
+  <si>
+    <t>19567</t>
+  </si>
+  <si>
+    <t>37628</t>
+  </si>
+  <si>
+    <t>51656</t>
+  </si>
+  <si>
+    <t>19568</t>
+  </si>
+  <si>
+    <t>37629</t>
+  </si>
+  <si>
+    <t>51657</t>
+  </si>
+  <si>
+    <t>19569</t>
+  </si>
+  <si>
+    <t>37632</t>
+  </si>
+  <si>
+    <t>51658</t>
+  </si>
+  <si>
+    <t>19570</t>
+  </si>
+  <si>
+    <t>37636</t>
+  </si>
+  <si>
+    <t>51659</t>
+  </si>
+  <si>
+    <t>19571</t>
+  </si>
+  <si>
+    <t>37639</t>
+  </si>
+  <si>
+    <t>51660</t>
+  </si>
+  <si>
+    <t>19572</t>
+  </si>
+  <si>
+    <t>37642</t>
+  </si>
+  <si>
+    <t>51661</t>
+  </si>
+  <si>
+    <t>19573</t>
+  </si>
+  <si>
+    <t>37644</t>
+  </si>
+  <si>
+    <t>51662</t>
+  </si>
+  <si>
+    <t>19574</t>
+  </si>
+  <si>
+    <t>37645</t>
+  </si>
+  <si>
+    <t>51663</t>
+  </si>
+  <si>
+    <t>19575</t>
+  </si>
+  <si>
+    <t>37646</t>
+  </si>
+  <si>
+    <t>51664</t>
+  </si>
+  <si>
+    <t>19576</t>
+  </si>
+  <si>
+    <t>37647</t>
+  </si>
+  <si>
+    <t>51665</t>
+  </si>
+  <si>
+    <t>19577</t>
+  </si>
+  <si>
+    <t>37648</t>
+  </si>
+  <si>
+    <t>51666</t>
+  </si>
+  <si>
+    <t>19578</t>
+  </si>
+  <si>
+    <t>37649</t>
+  </si>
+  <si>
+    <t>51667</t>
+  </si>
+  <si>
+    <t>19579</t>
+  </si>
+  <si>
+    <t>37650</t>
+  </si>
+  <si>
+    <t>Minimum AED 100,000 per member
+Out-patient: 20% coinsurance per visit
+Any type of organ transplantation is covered</t>
+  </si>
+  <si>
+    <t>51668</t>
+  </si>
+  <si>
+    <t>19580</t>
+  </si>
+  <si>
+    <t>37651</t>
+  </si>
+  <si>
+    <t>51669</t>
+  </si>
+  <si>
+    <t>19581</t>
+  </si>
+  <si>
+    <t>37652</t>
+  </si>
+  <si>
+    <t>51670</t>
+  </si>
+  <si>
+    <t>19582</t>
+  </si>
+  <si>
+    <t>37653</t>
+  </si>
+  <si>
+    <t>51671</t>
+  </si>
+  <si>
+    <t>19583</t>
+  </si>
+  <si>
+    <t>37654</t>
+  </si>
+  <si>
+    <t>51672</t>
+  </si>
+  <si>
+    <t>19584</t>
+  </si>
+  <si>
+    <t>37655</t>
+  </si>
+  <si>
+    <t>51673</t>
+  </si>
+  <si>
+    <t>19585</t>
+  </si>
+  <si>
+    <t>37660</t>
+  </si>
+  <si>
+    <t>51674</t>
+  </si>
+  <si>
+    <t>Dental Benefit</t>
+  </si>
+  <si>
+    <t>19586</t>
+  </si>
+  <si>
+    <t>37661</t>
+  </si>
+  <si>
+    <t>500</t>
+  </si>
+  <si>
+    <t>amount</t>
+  </si>
+  <si>
+    <t>Covered upto AED 500</t>
+  </si>
+  <si>
+    <t>51675</t>
+  </si>
+  <si>
+    <t>Dental Co-pay</t>
+  </si>
+  <si>
+    <t>19587</t>
+  </si>
+  <si>
+    <t>37667</t>
+  </si>
+  <si>
+    <t>30% co pay</t>
+  </si>
+  <si>
+    <t>Dental treatment Copay</t>
+  </si>
+  <si>
+    <t>51676</t>
+  </si>
+  <si>
+    <t>19592</t>
+  </si>
+  <si>
+    <t>37682</t>
+  </si>
+  <si>
+    <t>51677</t>
+  </si>
+  <si>
+    <t>19593</t>
+  </si>
+  <si>
+    <t>37683</t>
+  </si>
+  <si>
+    <t>51678</t>
+  </si>
+  <si>
+    <t>19594</t>
+  </si>
+  <si>
+    <t>37684</t>
+  </si>
+  <si>
+    <t>51679</t>
+  </si>
+  <si>
+    <t>19595</t>
+  </si>
+  <si>
+    <t>37685</t>
+  </si>
+  <si>
+    <t>51680</t>
+  </si>
+  <si>
+    <t>Dialysis</t>
+  </si>
+  <si>
+    <t>19597</t>
+  </si>
+  <si>
+    <t>37688</t>
+  </si>
+  <si>
+    <t>60000</t>
+  </si>
+  <si>
+    <t>Covered upto AED 60,000</t>
+  </si>
+  <si>
+    <t>51681</t>
+  </si>
+  <si>
+    <t>Virtual consultation</t>
+  </si>
+  <si>
+    <t>19599</t>
+  </si>
+  <si>
+    <t>37695</t>
+  </si>
+  <si>
+    <t>Covered
+20% coinsurance payable by the
+insured per visit
+No coinsurance if a follow-up visit
+made within seven days</t>
+  </si>
+  <si>
+    <t>51682</t>
+  </si>
+  <si>
+    <t>Disease Management Programme</t>
+  </si>
+  <si>
+    <t>19600</t>
+  </si>
+  <si>
+    <t>37696</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Covered
+</t>
+  </si>
+  <si>
+    <t>51683</t>
+  </si>
+  <si>
+    <t>Mental Health</t>
+  </si>
+  <si>
+    <t>19601</t>
+  </si>
+  <si>
+    <t>37697</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Outpatient counselling covered up to 800 per member. 
+30% coinsurance </t>
+  </si>
+  <si>
+    <t>55426</t>
+  </si>
+  <si>
+    <t>22214</t>
+  </si>
+  <si>
+    <t>42724</t>
+  </si>
+  <si>
+    <t>1698</t>
+  </si>
+  <si>
+    <t>TEST-ABC-0125-1-0119</t>
+  </si>
+  <si>
+    <t>55427</t>
+  </si>
+  <si>
+    <t>22215</t>
+  </si>
+  <si>
+    <t>42728</t>
+  </si>
+  <si>
+    <t>55428</t>
+  </si>
+  <si>
+    <t>22216</t>
+  </si>
+  <si>
+    <t>42729</t>
+  </si>
+  <si>
+    <t>55429</t>
+  </si>
+  <si>
+    <t>22217</t>
+  </si>
+  <si>
+    <t>42733</t>
+  </si>
+  <si>
+    <t>55430</t>
+  </si>
+  <si>
+    <t>22218</t>
+  </si>
+  <si>
+    <t>42734</t>
+  </si>
+  <si>
+    <t>55431</t>
+  </si>
+  <si>
+    <t>22219</t>
+  </si>
+  <si>
+    <t>42735</t>
+  </si>
+  <si>
+    <t>55432</t>
+  </si>
+  <si>
+    <t>22220</t>
+  </si>
+  <si>
+    <t>42736</t>
+  </si>
+  <si>
+    <t>55433</t>
+  </si>
+  <si>
+    <t>22221</t>
+  </si>
+  <si>
+    <t>42737</t>
+  </si>
+  <si>
+    <t>55434</t>
+  </si>
+  <si>
+    <t>22222</t>
+  </si>
+  <si>
+    <t>42738</t>
+  </si>
+  <si>
+    <t>55435</t>
+  </si>
+  <si>
+    <t>22223</t>
+  </si>
+  <si>
+    <t>42739</t>
+  </si>
+  <si>
+    <t>55436</t>
+  </si>
+  <si>
+    <t>22224</t>
+  </si>
+  <si>
+    <t>42740</t>
+  </si>
+  <si>
+    <t>55437</t>
+  </si>
+  <si>
+    <t>22225</t>
+  </si>
+  <si>
+    <t>42741</t>
+  </si>
+  <si>
+    <t>55438</t>
+  </si>
+  <si>
+    <t>22226</t>
+  </si>
+  <si>
+    <t>42744</t>
+  </si>
+  <si>
+    <t>55439</t>
+  </si>
+  <si>
+    <t>22227</t>
+  </si>
+  <si>
+    <t>42748</t>
+  </si>
+  <si>
+    <t>55440</t>
+  </si>
+  <si>
+    <t>22228</t>
+  </si>
+  <si>
+    <t>42751</t>
+  </si>
+  <si>
+    <t>55441</t>
+  </si>
+  <si>
+    <t>22229</t>
+  </si>
+  <si>
+    <t>42754</t>
+  </si>
+  <si>
+    <t>55442</t>
+  </si>
+  <si>
+    <t>Essential vaccinations for Children and Adults</t>
+  </si>
+  <si>
+    <t>22230</t>
+  </si>
+  <si>
+    <t>42756</t>
+  </si>
+  <si>
+    <t>55443</t>
+  </si>
+  <si>
+    <t>22231</t>
+  </si>
+  <si>
+    <t>42757</t>
+  </si>
+  <si>
+    <t>55444</t>
+  </si>
+  <si>
+    <t>22232</t>
+  </si>
+  <si>
+    <t>42758</t>
+  </si>
+  <si>
+    <t>55445</t>
+  </si>
+  <si>
+    <t>22233</t>
+  </si>
+  <si>
+    <t>42759</t>
+  </si>
+  <si>
+    <t>55446</t>
+  </si>
+  <si>
+    <t>22234</t>
+  </si>
+  <si>
+    <t>42760</t>
+  </si>
+  <si>
+    <t>55447</t>
+  </si>
+  <si>
+    <t>22235</t>
+  </si>
+  <si>
+    <t>42761</t>
+  </si>
+  <si>
+    <t>55448</t>
+  </si>
+  <si>
+    <t>22236</t>
+  </si>
+  <si>
+    <t>42762</t>
+  </si>
+  <si>
+    <t>55449</t>
+  </si>
+  <si>
+    <t>22237</t>
+  </si>
+  <si>
+    <t>42763</t>
+  </si>
+  <si>
+    <t>55450</t>
+  </si>
+  <si>
+    <t>22238</t>
+  </si>
+  <si>
+    <t>42764</t>
+  </si>
+  <si>
+    <t>55451</t>
+  </si>
+  <si>
+    <t>22239</t>
+  </si>
+  <si>
+    <t>42765</t>
+  </si>
+  <si>
+    <t>55452</t>
+  </si>
+  <si>
+    <t>22240</t>
+  </si>
+  <si>
+    <t>42766</t>
+  </si>
+  <si>
+    <t>55453</t>
+  </si>
+  <si>
+    <t>22241</t>
+  </si>
+  <si>
+    <t>42767</t>
+  </si>
+  <si>
+    <t>55454</t>
+  </si>
+  <si>
+    <t>22242</t>
+  </si>
+  <si>
+    <t>42772</t>
+  </si>
+  <si>
+    <t>55455</t>
+  </si>
+  <si>
+    <t>22243</t>
+  </si>
+  <si>
+    <t>42773</t>
+  </si>
+  <si>
+    <t>Dental Benefit
+Dental consultation, extraction, fillings, root canal treatment, scaling, x-rays, antibiotics and prophylaxis</t>
+  </si>
+  <si>
+    <t>Covered up to AED 500</t>
+  </si>
+  <si>
+    <t>55456</t>
+  </si>
+  <si>
+    <t>22244</t>
+  </si>
+  <si>
+    <t>42779</t>
+  </si>
+  <si>
+    <t>55457</t>
+  </si>
+  <si>
+    <t>22249</t>
+  </si>
+  <si>
+    <t>42794</t>
+  </si>
+  <si>
+    <t>55458</t>
+  </si>
+  <si>
+    <t>22250</t>
+  </si>
+  <si>
+    <t>42795</t>
+  </si>
+  <si>
+    <t>55459</t>
+  </si>
+  <si>
+    <t>22251</t>
+  </si>
+  <si>
+    <t>42796</t>
+  </si>
+  <si>
+    <t>55460</t>
+  </si>
+  <si>
+    <t>22252</t>
+  </si>
+  <si>
+    <t>42797</t>
+  </si>
+  <si>
+    <t>55461</t>
+  </si>
+  <si>
+    <t>22254</t>
+  </si>
+  <si>
+    <t>42800</t>
+  </si>
+  <si>
+    <t>Covered
+Minimum AED 60,000 per member
+Out-patient: 20% coinsurance per visit</t>
+  </si>
+  <si>
+    <t>55462</t>
+  </si>
+  <si>
+    <t>22256</t>
+  </si>
+  <si>
+    <t>42805</t>
+  </si>
+  <si>
+    <t>55463</t>
+  </si>
+  <si>
+    <t>22257</t>
+  </si>
+  <si>
+    <t>42806</t>
+  </si>
+  <si>
+    <t>55464</t>
+  </si>
+  <si>
+    <t>22258</t>
+  </si>
+  <si>
+    <t>42807</t>
   </si>
 </sst>
 </file>
@@ -42432,7 +43220,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{896EBE52-15E4-49E9-8AD1-C57995055998}">
-  <dimension ref="A1:Y34"/>
+  <dimension ref="A1:Y40"/>
   <sheetViews>
     <sheetView topLeftCell="G1" zoomScale="109" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -42547,16 +43335,16 @@
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" s="163" t="s">
-        <v>333</v>
+        <v>742</v>
       </c>
       <c r="B2" s="86" t="s">
         <v>42</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>334</v>
+        <v>743</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>335</v>
+        <v>744</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>245</v>
@@ -42565,13 +43353,13 @@
         <v>43</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>336</v>
+        <v>745</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>307</v>
+        <v>746</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>246</v>
@@ -42594,16 +43382,16 @@
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" s="163" t="s">
-        <v>338</v>
+        <v>747</v>
       </c>
       <c r="B3" s="86" t="s">
         <v>48</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>339</v>
+        <v>748</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>340</v>
+        <v>749</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>49</v>
@@ -42612,13 +43400,13 @@
         <v>43</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>336</v>
+        <v>745</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>307</v>
+        <v>746</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>246</v>
@@ -42641,16 +43429,16 @@
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A4" s="163" t="s">
-        <v>341</v>
+        <v>750</v>
       </c>
       <c r="B4" s="86" t="s">
         <v>50</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>342</v>
+        <v>751</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>343</v>
+        <v>752</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>51</v>
@@ -42659,13 +43447,13 @@
         <v>43</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>336</v>
+        <v>745</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>307</v>
+        <v>746</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>246</v>
@@ -42688,16 +43476,16 @@
     </row>
     <row r="5" spans="1:25" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="163" t="s">
-        <v>344</v>
+        <v>753</v>
       </c>
       <c r="B5" s="86" t="s">
         <v>52</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>345</v>
+        <v>754</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>346</v>
+        <v>755</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>521</v>
@@ -42706,13 +43494,13 @@
         <v>43</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>336</v>
+        <v>745</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>307</v>
+        <v>746</v>
       </c>
       <c r="J5" s="3" t="s">
         <v>246</v>
@@ -42735,16 +43523,16 @@
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A6" s="163" t="s">
-        <v>347</v>
+        <v>756</v>
       </c>
       <c r="B6" s="86" t="s">
         <v>53</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>348</v>
+        <v>757</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>349</v>
+        <v>758</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>522</v>
@@ -42753,13 +43541,13 @@
         <v>43</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>336</v>
+        <v>745</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>307</v>
+        <v>746</v>
       </c>
       <c r="J6" s="3" t="s">
         <v>246</v>
@@ -42782,16 +43570,16 @@
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A7" s="163" t="s">
-        <v>350</v>
+        <v>759</v>
       </c>
       <c r="B7" s="86" t="s">
         <v>54</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>351</v>
+        <v>760</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>352</v>
+        <v>761</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>55</v>
@@ -42800,13 +43588,13 @@
         <v>43</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>336</v>
+        <v>745</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>307</v>
+        <v>746</v>
       </c>
       <c r="J7" s="3" t="s">
         <v>246</v>
@@ -42829,16 +43617,16 @@
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A8" s="163" t="s">
-        <v>353</v>
+        <v>762</v>
       </c>
       <c r="B8" s="86" t="s">
         <v>57</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>354</v>
+        <v>763</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>355</v>
+        <v>764</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>58</v>
@@ -42847,13 +43635,13 @@
         <v>43</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>336</v>
+        <v>745</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>307</v>
+        <v>746</v>
       </c>
       <c r="J8" s="3" t="s">
         <v>246</v>
@@ -42876,16 +43664,16 @@
     </row>
     <row r="9" spans="1:25" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="163" t="s">
-        <v>356</v>
+        <v>765</v>
       </c>
       <c r="B9" s="86" t="s">
         <v>59</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>357</v>
+        <v>766</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>358</v>
+        <v>767</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>60</v>
@@ -42894,13 +43682,13 @@
         <v>43</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>336</v>
+        <v>745</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>307</v>
+        <v>746</v>
       </c>
       <c r="J9" s="3" t="s">
         <v>246</v>
@@ -42923,16 +43711,16 @@
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A10" s="163" t="s">
-        <v>359</v>
+        <v>768</v>
       </c>
       <c r="B10" s="86" t="s">
         <v>61</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>360</v>
+        <v>769</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>361</v>
+        <v>770</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>58</v>
@@ -42941,13 +43729,13 @@
         <v>43</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>336</v>
+        <v>745</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>307</v>
+        <v>746</v>
       </c>
       <c r="J10" s="3" t="s">
         <v>246</v>
@@ -42970,16 +43758,16 @@
     </row>
     <row r="11" spans="1:25" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" s="163" t="s">
-        <v>362</v>
+        <v>771</v>
       </c>
       <c r="B11" s="86" t="s">
         <v>62</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>363</v>
+        <v>772</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>364</v>
+        <v>773</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>60</v>
@@ -42988,13 +43776,13 @@
         <v>43</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>336</v>
+        <v>745</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>307</v>
+        <v>746</v>
       </c>
       <c r="J11" s="3" t="s">
         <v>246</v>
@@ -43017,16 +43805,16 @@
     </row>
     <row r="12" spans="1:25" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="163" t="s">
-        <v>365</v>
+        <v>774</v>
       </c>
       <c r="B12" s="86" t="s">
         <v>63</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>366</v>
+        <v>775</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>367</v>
+        <v>776</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>58</v>
@@ -43035,13 +43823,13 @@
         <v>43</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>336</v>
+        <v>745</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>307</v>
+        <v>746</v>
       </c>
       <c r="J12" s="3" t="s">
         <v>246</v>
@@ -43064,16 +43852,16 @@
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A13" s="163" t="s">
-        <v>368</v>
+        <v>777</v>
       </c>
       <c r="B13" s="86" t="s">
         <v>64</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>369</v>
+        <v>778</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>370</v>
+        <v>779</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>65</v>
@@ -43082,13 +43870,13 @@
         <v>43</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>336</v>
+        <v>745</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>307</v>
+        <v>746</v>
       </c>
       <c r="J13" s="3" t="s">
         <v>246</v>
@@ -43111,16 +43899,16 @@
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A14" s="163" t="s">
-        <v>371</v>
+        <v>780</v>
       </c>
       <c r="B14" s="86" t="s">
         <v>68</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>372</v>
+        <v>781</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>373</v>
+        <v>782</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>247</v>
@@ -43129,13 +43917,13 @@
         <v>43</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>336</v>
+        <v>745</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>307</v>
+        <v>746</v>
       </c>
       <c r="J14" s="3" t="s">
         <v>246</v>
@@ -43158,16 +43946,16 @@
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A15" s="163" t="s">
-        <v>374</v>
+        <v>783</v>
       </c>
       <c r="B15" s="86" t="s">
         <v>71</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>375</v>
+        <v>784</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>376</v>
+        <v>785</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>72</v>
@@ -43176,13 +43964,13 @@
         <v>43</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>336</v>
+        <v>745</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>307</v>
+        <v>746</v>
       </c>
       <c r="J15" s="3" t="s">
         <v>246</v>
@@ -43205,16 +43993,16 @@
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A16" s="163" t="s">
-        <v>377</v>
+        <v>786</v>
       </c>
       <c r="B16" s="86" t="s">
         <v>73</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>378</v>
+        <v>787</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>379</v>
+        <v>788</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>72</v>
@@ -43223,13 +44011,13 @@
         <v>43</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>336</v>
+        <v>745</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>307</v>
+        <v>746</v>
       </c>
       <c r="J16" s="3" t="s">
         <v>246</v>
@@ -43252,16 +44040,16 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="163" t="s">
-        <v>380</v>
+        <v>789</v>
       </c>
       <c r="B17" s="86" t="s">
         <v>75</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>381</v>
+        <v>790</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>382</v>
+        <v>791</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>76</v>
@@ -43270,13 +44058,13 @@
         <v>43</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>336</v>
+        <v>745</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>307</v>
+        <v>746</v>
       </c>
       <c r="J17" s="3" t="s">
         <v>246</v>
@@ -43299,16 +44087,16 @@
     </row>
     <row r="18" spans="1:15" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A18" s="163" t="s">
-        <v>383</v>
+        <v>792</v>
       </c>
       <c r="B18" s="86" t="s">
-        <v>78</v>
+        <v>793</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>384</v>
+        <v>794</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>385</v>
+        <v>795</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>79</v>
@@ -43317,13 +44105,13 @@
         <v>43</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>336</v>
+        <v>745</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>307</v>
+        <v>746</v>
       </c>
       <c r="J18" s="3" t="s">
         <v>246</v>
@@ -43335,7 +44123,7 @@
         <v>308</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>78</v>
+        <v>793</v>
       </c>
       <c r="N18" s="3" t="s">
         <v>79</v>
@@ -43346,16 +44134,16 @@
     </row>
     <row r="19" spans="1:15" ht="72" x14ac:dyDescent="0.3">
       <c r="A19" s="163" t="s">
-        <v>386</v>
+        <v>796</v>
       </c>
       <c r="B19" s="86" t="s">
         <v>523</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>387</v>
+        <v>797</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>388</v>
+        <v>798</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>81</v>
@@ -43364,13 +44152,13 @@
         <v>43</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>336</v>
+        <v>745</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>307</v>
+        <v>746</v>
       </c>
       <c r="J19" s="3" t="s">
         <v>246</v>
@@ -43393,16 +44181,16 @@
     </row>
     <row r="20" spans="1:15" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A20" s="163" t="s">
-        <v>389</v>
+        <v>799</v>
       </c>
       <c r="B20" s="86" t="s">
         <v>524</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>390</v>
+        <v>800</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>391</v>
+        <v>801</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>81</v>
@@ -43411,13 +44199,13 @@
         <v>43</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>336</v>
+        <v>745</v>
       </c>
       <c r="H20" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>307</v>
+        <v>746</v>
       </c>
       <c r="J20" s="3" t="s">
         <v>246</v>
@@ -43440,16 +44228,16 @@
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="163" t="s">
-        <v>392</v>
+        <v>802</v>
       </c>
       <c r="B21" s="86" t="s">
         <v>82</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>393</v>
+        <v>803</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>394</v>
+        <v>804</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>525</v>
@@ -43458,13 +44246,13 @@
         <v>43</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>336</v>
+        <v>745</v>
       </c>
       <c r="H21" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>307</v>
+        <v>746</v>
       </c>
       <c r="J21" s="3" t="s">
         <v>246</v>
@@ -43487,16 +44275,16 @@
     </row>
     <row r="22" spans="1:15" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A22" s="163" t="s">
-        <v>395</v>
+        <v>805</v>
       </c>
       <c r="B22" s="86" t="s">
         <v>526</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>396</v>
+        <v>806</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>397</v>
+        <v>807</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>83</v>
@@ -43505,13 +44293,13 @@
         <v>43</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>336</v>
+        <v>745</v>
       </c>
       <c r="H22" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>307</v>
+        <v>746</v>
       </c>
       <c r="J22" s="3" t="s">
         <v>246</v>
@@ -43534,16 +44322,16 @@
     </row>
     <row r="23" spans="1:15" ht="144" x14ac:dyDescent="0.3">
       <c r="A23" s="163" t="s">
-        <v>398</v>
+        <v>808</v>
       </c>
       <c r="B23" s="86" t="s">
         <v>527</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>399</v>
+        <v>809</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>400</v>
+        <v>810</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>83</v>
@@ -43552,13 +44340,13 @@
         <v>43</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>336</v>
+        <v>745</v>
       </c>
       <c r="H23" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>307</v>
+        <v>746</v>
       </c>
       <c r="J23" s="3" t="s">
         <v>246</v>
@@ -43581,16 +44369,16 @@
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" s="163" t="s">
-        <v>401</v>
+        <v>811</v>
       </c>
       <c r="B24" s="86" t="s">
         <v>84</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>402</v>
+        <v>812</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>403</v>
+        <v>813</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>58</v>
@@ -43599,13 +44387,13 @@
         <v>43</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>336</v>
+        <v>745</v>
       </c>
       <c r="H24" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>307</v>
+        <v>746</v>
       </c>
       <c r="J24" s="3" t="s">
         <v>246</v>
@@ -43620,7 +44408,7 @@
         <v>84</v>
       </c>
       <c r="N24" s="3" t="s">
-        <v>528</v>
+        <v>677</v>
       </c>
       <c r="O24" s="3" t="s">
         <v>80</v>
@@ -43628,16 +44416,16 @@
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" s="163" t="s">
-        <v>404</v>
+        <v>814</v>
       </c>
       <c r="B25" s="86" t="s">
         <v>85</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>405</v>
+        <v>815</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>406</v>
+        <v>816</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>86</v>
@@ -43646,13 +44434,13 @@
         <v>43</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>336</v>
+        <v>745</v>
       </c>
       <c r="H25" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>307</v>
+        <v>746</v>
       </c>
       <c r="J25" s="3" t="s">
         <v>246</v>
@@ -43675,16 +44463,16 @@
     </row>
     <row r="26" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="163" t="s">
-        <v>407</v>
+        <v>817</v>
       </c>
       <c r="B26" s="86" t="s">
         <v>88</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>408</v>
+        <v>818</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>409</v>
+        <v>819</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>89</v>
@@ -43693,13 +44481,13 @@
         <v>43</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>336</v>
+        <v>745</v>
       </c>
       <c r="H26" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>307</v>
+        <v>746</v>
       </c>
       <c r="J26" s="3" t="s">
         <v>246</v>
@@ -43722,16 +44510,16 @@
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" s="163" t="s">
-        <v>410</v>
+        <v>820</v>
       </c>
       <c r="B27" s="86" t="s">
         <v>90</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>411</v>
+        <v>821</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>412</v>
+        <v>822</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>58</v>
@@ -43740,13 +44528,13 @@
         <v>43</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>336</v>
+        <v>745</v>
       </c>
       <c r="H27" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>307</v>
+        <v>746</v>
       </c>
       <c r="J27" s="3" t="s">
         <v>246</v>
@@ -43769,16 +44557,16 @@
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" s="163" t="s">
-        <v>413</v>
+        <v>823</v>
       </c>
       <c r="B28" s="86" t="s">
         <v>91</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>414</v>
+        <v>824</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>415</v>
+        <v>825</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>92</v>
@@ -43787,13 +44575,13 @@
         <v>43</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>336</v>
+        <v>745</v>
       </c>
       <c r="H28" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>307</v>
+        <v>746</v>
       </c>
       <c r="J28" s="3" t="s">
         <v>246</v>
@@ -43816,16 +44604,16 @@
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" s="163" t="s">
-        <v>416</v>
+        <v>826</v>
       </c>
       <c r="B29" s="86" t="s">
         <v>95</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>417</v>
+        <v>827</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>418</v>
+        <v>828</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>248</v>
@@ -43834,13 +44622,13 @@
         <v>43</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>336</v>
+        <v>745</v>
       </c>
       <c r="H29" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>307</v>
+        <v>746</v>
       </c>
       <c r="J29" s="3" t="s">
         <v>246</v>
@@ -43863,16 +44651,16 @@
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" s="163" t="s">
-        <v>419</v>
+        <v>829</v>
       </c>
       <c r="B30" s="86" t="s">
         <v>98</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>420</v>
+        <v>830</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>421</v>
+        <v>831</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>58</v>
@@ -43881,13 +44669,13 @@
         <v>43</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>336</v>
+        <v>745</v>
       </c>
       <c r="H30" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>307</v>
+        <v>746</v>
       </c>
       <c r="J30" s="3" t="s">
         <v>246</v>
@@ -43910,78 +44698,78 @@
     </row>
     <row r="31" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="163" t="s">
-        <v>422</v>
+        <v>832</v>
       </c>
       <c r="B31" s="86" t="s">
-        <v>531</v>
+        <v>697</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>423</v>
+        <v>833</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>424</v>
+        <v>834</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>100</v>
+        <v>700</v>
       </c>
       <c r="F31" s="3" t="s">
         <v>43</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>336</v>
+        <v>745</v>
       </c>
       <c r="H31" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>307</v>
+        <v>746</v>
       </c>
       <c r="J31" s="3" t="s">
         <v>246</v>
       </c>
       <c r="K31" s="3" t="s">
-        <v>45</v>
+        <v>701</v>
       </c>
       <c r="L31" s="3" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="M31" s="3" t="s">
-        <v>531</v>
+        <v>835</v>
       </c>
       <c r="N31" s="3" t="s">
-        <v>100</v>
+        <v>836</v>
       </c>
       <c r="O31" s="3" t="s">
-        <v>101</v>
+        <v>80</v>
       </c>
     </row>
     <row r="32" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="163" t="s">
-        <v>425</v>
+        <v>837</v>
       </c>
       <c r="B32" s="86" t="s">
-        <v>102</v>
+        <v>704</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>426</v>
+        <v>838</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>427</v>
+        <v>839</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>103</v>
+        <v>707</v>
       </c>
       <c r="F32" s="3" t="s">
         <v>43</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>336</v>
+        <v>745</v>
       </c>
       <c r="H32" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>307</v>
+        <v>746</v>
       </c>
       <c r="J32" s="3" t="s">
         <v>246</v>
@@ -43990,45 +44778,45 @@
         <v>45</v>
       </c>
       <c r="L32" s="3" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="M32" s="3" t="s">
-        <v>102</v>
+        <v>708</v>
       </c>
       <c r="N32" s="3" t="s">
-        <v>103</v>
+        <v>707</v>
       </c>
       <c r="O32" s="3" t="s">
-        <v>101</v>
+        <v>80</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" s="163" t="s">
-        <v>428</v>
+        <v>840</v>
       </c>
       <c r="B33" s="86" t="s">
-        <v>104</v>
+        <v>531</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>429</v>
+        <v>841</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>430</v>
+        <v>842</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="F33" s="3" t="s">
         <v>43</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>336</v>
+        <v>745</v>
       </c>
       <c r="H33" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>307</v>
+        <v>746</v>
       </c>
       <c r="J33" s="3" t="s">
         <v>246</v>
@@ -44040,10 +44828,10 @@
         <v>308</v>
       </c>
       <c r="M33" s="3" t="s">
-        <v>104</v>
+        <v>531</v>
       </c>
       <c r="N33" s="3" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="O33" s="3" t="s">
         <v>101</v>
@@ -44051,31 +44839,31 @@
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34" s="163" t="s">
-        <v>431</v>
+        <v>843</v>
       </c>
       <c r="B34" s="86" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>432</v>
+        <v>844</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>433</v>
+        <v>845</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="F34" s="3" t="s">
         <v>43</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>336</v>
+        <v>745</v>
       </c>
       <c r="H34" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>307</v>
+        <v>746</v>
       </c>
       <c r="J34" s="3" t="s">
         <v>246</v>
@@ -44087,12 +44875,294 @@
         <v>308</v>
       </c>
       <c r="M34" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="N34" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="O34" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s" s="163">
+        <v>846</v>
+      </c>
+      <c r="B35" t="s" s="86">
+        <v>104</v>
+      </c>
+      <c r="C35" t="s" s="3">
+        <v>847</v>
+      </c>
+      <c r="D35" t="s" s="3">
+        <v>848</v>
+      </c>
+      <c r="E35" t="s" s="3">
+        <v>105</v>
+      </c>
+      <c r="F35" t="s" s="3">
+        <v>43</v>
+      </c>
+      <c r="G35" t="s" s="3">
+        <v>745</v>
+      </c>
+      <c r="H35" t="s" s="3">
+        <v>337</v>
+      </c>
+      <c r="I35" t="s" s="3">
+        <v>746</v>
+      </c>
+      <c r="J35" t="s" s="3">
+        <v>246</v>
+      </c>
+      <c r="K35" t="s" s="3">
+        <v>45</v>
+      </c>
+      <c r="L35" t="s" s="3">
+        <v>308</v>
+      </c>
+      <c r="M35" t="s" s="3">
+        <v>104</v>
+      </c>
+      <c r="N35" t="s" s="3">
+        <v>105</v>
+      </c>
+      <c r="O35" t="s" s="3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s" s="163">
+        <v>849</v>
+      </c>
+      <c r="B36" t="s" s="86">
         <v>106</v>
       </c>
-      <c r="N34" s="3" t="s">
+      <c r="C36" t="s" s="3">
+        <v>850</v>
+      </c>
+      <c r="D36" t="s" s="3">
+        <v>851</v>
+      </c>
+      <c r="E36" t="s" s="3">
         <v>107</v>
       </c>
-      <c r="O34" s="3" t="s">
+      <c r="F36" t="s" s="3">
+        <v>43</v>
+      </c>
+      <c r="G36" t="s" s="3">
+        <v>745</v>
+      </c>
+      <c r="H36" t="s" s="3">
+        <v>337</v>
+      </c>
+      <c r="I36" t="s" s="3">
+        <v>746</v>
+      </c>
+      <c r="J36" t="s" s="3">
+        <v>246</v>
+      </c>
+      <c r="K36" t="s" s="3">
+        <v>45</v>
+      </c>
+      <c r="L36" t="s" s="3">
+        <v>308</v>
+      </c>
+      <c r="M36" t="s" s="3">
+        <v>106</v>
+      </c>
+      <c r="N36" t="s" s="3">
+        <v>107</v>
+      </c>
+      <c r="O36" t="s" s="3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s" s="163">
+        <v>852</v>
+      </c>
+      <c r="B37" t="s" s="86">
+        <v>722</v>
+      </c>
+      <c r="C37" t="s" s="3">
+        <v>853</v>
+      </c>
+      <c r="D37" t="s" s="3">
+        <v>854</v>
+      </c>
+      <c r="E37" t="s" s="3">
+        <v>855</v>
+      </c>
+      <c r="F37" t="s" s="3">
+        <v>43</v>
+      </c>
+      <c r="G37" t="s" s="3">
+        <v>745</v>
+      </c>
+      <c r="H37" t="s" s="3">
+        <v>337</v>
+      </c>
+      <c r="I37" t="s" s="3">
+        <v>746</v>
+      </c>
+      <c r="J37" t="s" s="3">
+        <v>246</v>
+      </c>
+      <c r="K37" t="s" s="3">
+        <v>45</v>
+      </c>
+      <c r="L37" t="s" s="3">
+        <v>310</v>
+      </c>
+      <c r="M37" t="s" s="3">
+        <v>722</v>
+      </c>
+      <c r="N37" t="s" s="3">
+        <v>855</v>
+      </c>
+      <c r="O37" t="s" s="3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s" s="163">
+        <v>856</v>
+      </c>
+      <c r="B38" t="s" s="86">
+        <v>728</v>
+      </c>
+      <c r="C38" t="s" s="3">
+        <v>857</v>
+      </c>
+      <c r="D38" t="s" s="3">
+        <v>858</v>
+      </c>
+      <c r="E38" t="s" s="3">
+        <v>731</v>
+      </c>
+      <c r="F38" t="s" s="3">
+        <v>43</v>
+      </c>
+      <c r="G38" t="s" s="3">
+        <v>745</v>
+      </c>
+      <c r="H38" t="s" s="3">
+        <v>337</v>
+      </c>
+      <c r="I38" t="s" s="3">
+        <v>746</v>
+      </c>
+      <c r="J38" t="s" s="3">
+        <v>246</v>
+      </c>
+      <c r="K38" t="s" s="3">
+        <v>45</v>
+      </c>
+      <c r="L38" t="s" s="3">
+        <v>308</v>
+      </c>
+      <c r="M38" t="s" s="3">
+        <v>728</v>
+      </c>
+      <c r="N38" t="s" s="3">
+        <v>731</v>
+      </c>
+      <c r="O38" t="s" s="3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s" s="163">
+        <v>859</v>
+      </c>
+      <c r="B39" t="s" s="86">
+        <v>733</v>
+      </c>
+      <c r="C39" t="s" s="3">
+        <v>860</v>
+      </c>
+      <c r="D39" t="s" s="3">
+        <v>861</v>
+      </c>
+      <c r="E39" t="s" s="3">
+        <v>736</v>
+      </c>
+      <c r="F39" t="s" s="3">
+        <v>43</v>
+      </c>
+      <c r="G39" t="s" s="3">
+        <v>745</v>
+      </c>
+      <c r="H39" t="s" s="3">
+        <v>337</v>
+      </c>
+      <c r="I39" t="s" s="3">
+        <v>746</v>
+      </c>
+      <c r="J39" t="s" s="3">
+        <v>246</v>
+      </c>
+      <c r="K39" t="s" s="3">
+        <v>45</v>
+      </c>
+      <c r="L39" t="s" s="3">
+        <v>308</v>
+      </c>
+      <c r="M39" t="s" s="3">
+        <v>733</v>
+      </c>
+      <c r="N39" t="s" s="3">
+        <v>736</v>
+      </c>
+      <c r="O39" t="s" s="3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s" s="163">
+        <v>862</v>
+      </c>
+      <c r="B40" t="s" s="86">
+        <v>738</v>
+      </c>
+      <c r="C40" t="s" s="3">
+        <v>863</v>
+      </c>
+      <c r="D40" t="s" s="3">
+        <v>864</v>
+      </c>
+      <c r="E40" t="s" s="3">
+        <v>741</v>
+      </c>
+      <c r="F40" t="s" s="3">
+        <v>43</v>
+      </c>
+      <c r="G40" t="s" s="3">
+        <v>745</v>
+      </c>
+      <c r="H40" t="s" s="3">
+        <v>337</v>
+      </c>
+      <c r="I40" t="s" s="3">
+        <v>746</v>
+      </c>
+      <c r="J40" t="s" s="3">
+        <v>246</v>
+      </c>
+      <c r="K40" t="s" s="3">
+        <v>45</v>
+      </c>
+      <c r="L40" t="s" s="3">
+        <v>308</v>
+      </c>
+      <c r="M40" t="s" s="3">
+        <v>738</v>
+      </c>
+      <c r="N40" t="s" s="3">
+        <v>741</v>
+      </c>
+      <c r="O40" t="s" s="3">
         <v>80</v>
       </c>
     </row>

</xml_diff>

<commit_message>
final code of calculation create qoute aiaw
</commit_message>
<xml_diff>
--- a/target/ExcelCalculatorForDistributor/Arshad New Calculator.xlsx
+++ b/target/ExcelCalculatorForDistributor/Arshad New Calculator.xlsx
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42443" uniqueCount="865">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52283" uniqueCount="1111">
   <si>
     <t>id</t>
   </si>
@@ -2761,6 +2761,744 @@
   </si>
   <si>
     <t>42807</t>
+  </si>
+  <si>
+    <t>55465</t>
+  </si>
+  <si>
+    <t>1699</t>
+  </si>
+  <si>
+    <t>TEST-ABC-0125-1-0120</t>
+  </si>
+  <si>
+    <t>55466</t>
+  </si>
+  <si>
+    <t>55467</t>
+  </si>
+  <si>
+    <t>55468</t>
+  </si>
+  <si>
+    <t>55469</t>
+  </si>
+  <si>
+    <t>55470</t>
+  </si>
+  <si>
+    <t>55471</t>
+  </si>
+  <si>
+    <t>55472</t>
+  </si>
+  <si>
+    <t>55473</t>
+  </si>
+  <si>
+    <t>55474</t>
+  </si>
+  <si>
+    <t>55475</t>
+  </si>
+  <si>
+    <t>55476</t>
+  </si>
+  <si>
+    <t>55477</t>
+  </si>
+  <si>
+    <t>55478</t>
+  </si>
+  <si>
+    <t>55479</t>
+  </si>
+  <si>
+    <t>55480</t>
+  </si>
+  <si>
+    <t>55481</t>
+  </si>
+  <si>
+    <t>55482</t>
+  </si>
+  <si>
+    <t>55483</t>
+  </si>
+  <si>
+    <t>55484</t>
+  </si>
+  <si>
+    <t>55485</t>
+  </si>
+  <si>
+    <t>55486</t>
+  </si>
+  <si>
+    <t>55487</t>
+  </si>
+  <si>
+    <t>55488</t>
+  </si>
+  <si>
+    <t>55489</t>
+  </si>
+  <si>
+    <t>55490</t>
+  </si>
+  <si>
+    <t>55491</t>
+  </si>
+  <si>
+    <t>55492</t>
+  </si>
+  <si>
+    <t>55493</t>
+  </si>
+  <si>
+    <t>55494</t>
+  </si>
+  <si>
+    <t>55495</t>
+  </si>
+  <si>
+    <t>55496</t>
+  </si>
+  <si>
+    <t>55497</t>
+  </si>
+  <si>
+    <t>55498</t>
+  </si>
+  <si>
+    <t>55499</t>
+  </si>
+  <si>
+    <t>55500</t>
+  </si>
+  <si>
+    <t>55501</t>
+  </si>
+  <si>
+    <t>55502</t>
+  </si>
+  <si>
+    <t>55503</t>
+  </si>
+  <si>
+    <t>55504</t>
+  </si>
+  <si>
+    <t>1700</t>
+  </si>
+  <si>
+    <t>TEST-ABC-0125-1-0121</t>
+  </si>
+  <si>
+    <t>55505</t>
+  </si>
+  <si>
+    <t>55506</t>
+  </si>
+  <si>
+    <t>55507</t>
+  </si>
+  <si>
+    <t>55508</t>
+  </si>
+  <si>
+    <t>55509</t>
+  </si>
+  <si>
+    <t>55510</t>
+  </si>
+  <si>
+    <t>55511</t>
+  </si>
+  <si>
+    <t>55512</t>
+  </si>
+  <si>
+    <t>55513</t>
+  </si>
+  <si>
+    <t>55514</t>
+  </si>
+  <si>
+    <t>55515</t>
+  </si>
+  <si>
+    <t>55516</t>
+  </si>
+  <si>
+    <t>55517</t>
+  </si>
+  <si>
+    <t>55518</t>
+  </si>
+  <si>
+    <t>55519</t>
+  </si>
+  <si>
+    <t>55520</t>
+  </si>
+  <si>
+    <t>55521</t>
+  </si>
+  <si>
+    <t>55522</t>
+  </si>
+  <si>
+    <t>55523</t>
+  </si>
+  <si>
+    <t>55524</t>
+  </si>
+  <si>
+    <t>55525</t>
+  </si>
+  <si>
+    <t>55526</t>
+  </si>
+  <si>
+    <t>55527</t>
+  </si>
+  <si>
+    <t>55528</t>
+  </si>
+  <si>
+    <t>55529</t>
+  </si>
+  <si>
+    <t>55530</t>
+  </si>
+  <si>
+    <t>55531</t>
+  </si>
+  <si>
+    <t>55532</t>
+  </si>
+  <si>
+    <t>55533</t>
+  </si>
+  <si>
+    <t>55534</t>
+  </si>
+  <si>
+    <t>55535</t>
+  </si>
+  <si>
+    <t>55536</t>
+  </si>
+  <si>
+    <t>55537</t>
+  </si>
+  <si>
+    <t>55538</t>
+  </si>
+  <si>
+    <t>55539</t>
+  </si>
+  <si>
+    <t>55540</t>
+  </si>
+  <si>
+    <t>55541</t>
+  </si>
+  <si>
+    <t>55542</t>
+  </si>
+  <si>
+    <t>55543</t>
+  </si>
+  <si>
+    <t>1701</t>
+  </si>
+  <si>
+    <t>TEST-ABC-0125-1-0122</t>
+  </si>
+  <si>
+    <t>55544</t>
+  </si>
+  <si>
+    <t>55545</t>
+  </si>
+  <si>
+    <t>55546</t>
+  </si>
+  <si>
+    <t>55547</t>
+  </si>
+  <si>
+    <t>55548</t>
+  </si>
+  <si>
+    <t>55549</t>
+  </si>
+  <si>
+    <t>55550</t>
+  </si>
+  <si>
+    <t>55551</t>
+  </si>
+  <si>
+    <t>55552</t>
+  </si>
+  <si>
+    <t>55553</t>
+  </si>
+  <si>
+    <t>55554</t>
+  </si>
+  <si>
+    <t>55555</t>
+  </si>
+  <si>
+    <t>55556</t>
+  </si>
+  <si>
+    <t>55557</t>
+  </si>
+  <si>
+    <t>55558</t>
+  </si>
+  <si>
+    <t>55559</t>
+  </si>
+  <si>
+    <t>55560</t>
+  </si>
+  <si>
+    <t>55561</t>
+  </si>
+  <si>
+    <t>55562</t>
+  </si>
+  <si>
+    <t>55563</t>
+  </si>
+  <si>
+    <t>55564</t>
+  </si>
+  <si>
+    <t>55565</t>
+  </si>
+  <si>
+    <t>55566</t>
+  </si>
+  <si>
+    <t>55567</t>
+  </si>
+  <si>
+    <t>55568</t>
+  </si>
+  <si>
+    <t>55569</t>
+  </si>
+  <si>
+    <t>55570</t>
+  </si>
+  <si>
+    <t>55571</t>
+  </si>
+  <si>
+    <t>55572</t>
+  </si>
+  <si>
+    <t>55573</t>
+  </si>
+  <si>
+    <t>55574</t>
+  </si>
+  <si>
+    <t>55575</t>
+  </si>
+  <si>
+    <t>55576</t>
+  </si>
+  <si>
+    <t>55577</t>
+  </si>
+  <si>
+    <t>55578</t>
+  </si>
+  <si>
+    <t>55579</t>
+  </si>
+  <si>
+    <t>55580</t>
+  </si>
+  <si>
+    <t>55581</t>
+  </si>
+  <si>
+    <t>55582</t>
+  </si>
+  <si>
+    <t>1702</t>
+  </si>
+  <si>
+    <t>TEST-ABC-0125-1-0123</t>
+  </si>
+  <si>
+    <t>55583</t>
+  </si>
+  <si>
+    <t>55584</t>
+  </si>
+  <si>
+    <t>55585</t>
+  </si>
+  <si>
+    <t>55586</t>
+  </si>
+  <si>
+    <t>55587</t>
+  </si>
+  <si>
+    <t>55588</t>
+  </si>
+  <si>
+    <t>55589</t>
+  </si>
+  <si>
+    <t>55590</t>
+  </si>
+  <si>
+    <t>55591</t>
+  </si>
+  <si>
+    <t>55592</t>
+  </si>
+  <si>
+    <t>55593</t>
+  </si>
+  <si>
+    <t>55594</t>
+  </si>
+  <si>
+    <t>55595</t>
+  </si>
+  <si>
+    <t>55596</t>
+  </si>
+  <si>
+    <t>55597</t>
+  </si>
+  <si>
+    <t>55598</t>
+  </si>
+  <si>
+    <t>55599</t>
+  </si>
+  <si>
+    <t>55600</t>
+  </si>
+  <si>
+    <t>55601</t>
+  </si>
+  <si>
+    <t>55602</t>
+  </si>
+  <si>
+    <t>55603</t>
+  </si>
+  <si>
+    <t>55604</t>
+  </si>
+  <si>
+    <t>55605</t>
+  </si>
+  <si>
+    <t>55606</t>
+  </si>
+  <si>
+    <t>55607</t>
+  </si>
+  <si>
+    <t>55608</t>
+  </si>
+  <si>
+    <t>55609</t>
+  </si>
+  <si>
+    <t>55610</t>
+  </si>
+  <si>
+    <t>55611</t>
+  </si>
+  <si>
+    <t>55612</t>
+  </si>
+  <si>
+    <t>55613</t>
+  </si>
+  <si>
+    <t>55614</t>
+  </si>
+  <si>
+    <t>55615</t>
+  </si>
+  <si>
+    <t>55616</t>
+  </si>
+  <si>
+    <t>55617</t>
+  </si>
+  <si>
+    <t>55618</t>
+  </si>
+  <si>
+    <t>55619</t>
+  </si>
+  <si>
+    <t>55620</t>
+  </si>
+  <si>
+    <t>55621</t>
+  </si>
+  <si>
+    <t>1703</t>
+  </si>
+  <si>
+    <t>TEST-ABC-0125-1-0124</t>
+  </si>
+  <si>
+    <t>55622</t>
+  </si>
+  <si>
+    <t>55623</t>
+  </si>
+  <si>
+    <t>55624</t>
+  </si>
+  <si>
+    <t>55625</t>
+  </si>
+  <si>
+    <t>55626</t>
+  </si>
+  <si>
+    <t>55627</t>
+  </si>
+  <si>
+    <t>55628</t>
+  </si>
+  <si>
+    <t>55629</t>
+  </si>
+  <si>
+    <t>55630</t>
+  </si>
+  <si>
+    <t>55631</t>
+  </si>
+  <si>
+    <t>55632</t>
+  </si>
+  <si>
+    <t>55633</t>
+  </si>
+  <si>
+    <t>55634</t>
+  </si>
+  <si>
+    <t>55635</t>
+  </si>
+  <si>
+    <t>55636</t>
+  </si>
+  <si>
+    <t>55637</t>
+  </si>
+  <si>
+    <t>55638</t>
+  </si>
+  <si>
+    <t>55639</t>
+  </si>
+  <si>
+    <t>55640</t>
+  </si>
+  <si>
+    <t>55641</t>
+  </si>
+  <si>
+    <t>55642</t>
+  </si>
+  <si>
+    <t>55643</t>
+  </si>
+  <si>
+    <t>55644</t>
+  </si>
+  <si>
+    <t>55645</t>
+  </si>
+  <si>
+    <t>55646</t>
+  </si>
+  <si>
+    <t>55647</t>
+  </si>
+  <si>
+    <t>55648</t>
+  </si>
+  <si>
+    <t>55649</t>
+  </si>
+  <si>
+    <t>55650</t>
+  </si>
+  <si>
+    <t>55651</t>
+  </si>
+  <si>
+    <t>55652</t>
+  </si>
+  <si>
+    <t>55653</t>
+  </si>
+  <si>
+    <t>55654</t>
+  </si>
+  <si>
+    <t>55655</t>
+  </si>
+  <si>
+    <t>55656</t>
+  </si>
+  <si>
+    <t>55657</t>
+  </si>
+  <si>
+    <t>55658</t>
+  </si>
+  <si>
+    <t>55659</t>
+  </si>
+  <si>
+    <t>55706</t>
+  </si>
+  <si>
+    <t>1705</t>
+  </si>
+  <si>
+    <t>TEST-ABC-0125-1-0126</t>
+  </si>
+  <si>
+    <t>55707</t>
+  </si>
+  <si>
+    <t>55708</t>
+  </si>
+  <si>
+    <t>55709</t>
+  </si>
+  <si>
+    <t>55710</t>
+  </si>
+  <si>
+    <t>55711</t>
+  </si>
+  <si>
+    <t>55712</t>
+  </si>
+  <si>
+    <t>55713</t>
+  </si>
+  <si>
+    <t>55714</t>
+  </si>
+  <si>
+    <t>55715</t>
+  </si>
+  <si>
+    <t>55716</t>
+  </si>
+  <si>
+    <t>55717</t>
+  </si>
+  <si>
+    <t>55718</t>
+  </si>
+  <si>
+    <t>55719</t>
+  </si>
+  <si>
+    <t>55720</t>
+  </si>
+  <si>
+    <t>55721</t>
+  </si>
+  <si>
+    <t>55722</t>
+  </si>
+  <si>
+    <t>55723</t>
+  </si>
+  <si>
+    <t>55724</t>
+  </si>
+  <si>
+    <t>55725</t>
+  </si>
+  <si>
+    <t>55726</t>
+  </si>
+  <si>
+    <t>55727</t>
+  </si>
+  <si>
+    <t>55728</t>
+  </si>
+  <si>
+    <t>55729</t>
+  </si>
+  <si>
+    <t>55730</t>
+  </si>
+  <si>
+    <t>55731</t>
+  </si>
+  <si>
+    <t>55732</t>
+  </si>
+  <si>
+    <t>55733</t>
+  </si>
+  <si>
+    <t>55734</t>
+  </si>
+  <si>
+    <t>55735</t>
+  </si>
+  <si>
+    <t>55736</t>
+  </si>
+  <si>
+    <t>55737</t>
+  </si>
+  <si>
+    <t>55738</t>
+  </si>
+  <si>
+    <t>55739</t>
+  </si>
+  <si>
+    <t>55740</t>
+  </si>
+  <si>
+    <t>55741</t>
+  </si>
+  <si>
+    <t>55742</t>
+  </si>
+  <si>
+    <t>55743</t>
+  </si>
+  <si>
+    <t>55744</t>
   </si>
 </sst>
 </file>
@@ -43335,7 +44073,7 @@
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" s="163" t="s">
-        <v>742</v>
+        <v>1070</v>
       </c>
       <c r="B2" s="86" t="s">
         <v>42</v>
@@ -43353,13 +44091,13 @@
         <v>43</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>745</v>
+        <v>1071</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>746</v>
+        <v>1072</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>246</v>
@@ -43382,7 +44120,7 @@
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" s="163" t="s">
-        <v>747</v>
+        <v>1073</v>
       </c>
       <c r="B3" s="86" t="s">
         <v>48</v>
@@ -43400,13 +44138,13 @@
         <v>43</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>745</v>
+        <v>1071</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>746</v>
+        <v>1072</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>246</v>
@@ -43429,7 +44167,7 @@
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A4" s="163" t="s">
-        <v>750</v>
+        <v>1074</v>
       </c>
       <c r="B4" s="86" t="s">
         <v>50</v>
@@ -43447,13 +44185,13 @@
         <v>43</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>745</v>
+        <v>1071</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>746</v>
+        <v>1072</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>246</v>
@@ -43476,7 +44214,7 @@
     </row>
     <row r="5" spans="1:25" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="163" t="s">
-        <v>753</v>
+        <v>1075</v>
       </c>
       <c r="B5" s="86" t="s">
         <v>52</v>
@@ -43494,13 +44232,13 @@
         <v>43</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>745</v>
+        <v>1071</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>746</v>
+        <v>1072</v>
       </c>
       <c r="J5" s="3" t="s">
         <v>246</v>
@@ -43523,7 +44261,7 @@
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A6" s="163" t="s">
-        <v>756</v>
+        <v>1076</v>
       </c>
       <c r="B6" s="86" t="s">
         <v>53</v>
@@ -43541,13 +44279,13 @@
         <v>43</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>745</v>
+        <v>1071</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>746</v>
+        <v>1072</v>
       </c>
       <c r="J6" s="3" t="s">
         <v>246</v>
@@ -43570,7 +44308,7 @@
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A7" s="163" t="s">
-        <v>759</v>
+        <v>1077</v>
       </c>
       <c r="B7" s="86" t="s">
         <v>54</v>
@@ -43588,13 +44326,13 @@
         <v>43</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>745</v>
+        <v>1071</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>746</v>
+        <v>1072</v>
       </c>
       <c r="J7" s="3" t="s">
         <v>246</v>
@@ -43617,7 +44355,7 @@
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A8" s="163" t="s">
-        <v>762</v>
+        <v>1078</v>
       </c>
       <c r="B8" s="86" t="s">
         <v>57</v>
@@ -43635,13 +44373,13 @@
         <v>43</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>745</v>
+        <v>1071</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>746</v>
+        <v>1072</v>
       </c>
       <c r="J8" s="3" t="s">
         <v>246</v>
@@ -43664,7 +44402,7 @@
     </row>
     <row r="9" spans="1:25" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="163" t="s">
-        <v>765</v>
+        <v>1079</v>
       </c>
       <c r="B9" s="86" t="s">
         <v>59</v>
@@ -43682,13 +44420,13 @@
         <v>43</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>745</v>
+        <v>1071</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>746</v>
+        <v>1072</v>
       </c>
       <c r="J9" s="3" t="s">
         <v>246</v>
@@ -43711,7 +44449,7 @@
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A10" s="163" t="s">
-        <v>768</v>
+        <v>1080</v>
       </c>
       <c r="B10" s="86" t="s">
         <v>61</v>
@@ -43729,13 +44467,13 @@
         <v>43</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>745</v>
+        <v>1071</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>746</v>
+        <v>1072</v>
       </c>
       <c r="J10" s="3" t="s">
         <v>246</v>
@@ -43758,7 +44496,7 @@
     </row>
     <row r="11" spans="1:25" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" s="163" t="s">
-        <v>771</v>
+        <v>1081</v>
       </c>
       <c r="B11" s="86" t="s">
         <v>62</v>
@@ -43776,13 +44514,13 @@
         <v>43</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>745</v>
+        <v>1071</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>746</v>
+        <v>1072</v>
       </c>
       <c r="J11" s="3" t="s">
         <v>246</v>
@@ -43805,7 +44543,7 @@
     </row>
     <row r="12" spans="1:25" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="163" t="s">
-        <v>774</v>
+        <v>1082</v>
       </c>
       <c r="B12" s="86" t="s">
         <v>63</v>
@@ -43823,13 +44561,13 @@
         <v>43</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>745</v>
+        <v>1071</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>746</v>
+        <v>1072</v>
       </c>
       <c r="J12" s="3" t="s">
         <v>246</v>
@@ -43852,7 +44590,7 @@
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A13" s="163" t="s">
-        <v>777</v>
+        <v>1083</v>
       </c>
       <c r="B13" s="86" t="s">
         <v>64</v>
@@ -43870,13 +44608,13 @@
         <v>43</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>745</v>
+        <v>1071</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>746</v>
+        <v>1072</v>
       </c>
       <c r="J13" s="3" t="s">
         <v>246</v>
@@ -43899,7 +44637,7 @@
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A14" s="163" t="s">
-        <v>780</v>
+        <v>1084</v>
       </c>
       <c r="B14" s="86" t="s">
         <v>68</v>
@@ -43917,13 +44655,13 @@
         <v>43</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>745</v>
+        <v>1071</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>746</v>
+        <v>1072</v>
       </c>
       <c r="J14" s="3" t="s">
         <v>246</v>
@@ -43946,7 +44684,7 @@
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A15" s="163" t="s">
-        <v>783</v>
+        <v>1085</v>
       </c>
       <c r="B15" s="86" t="s">
         <v>71</v>
@@ -43964,13 +44702,13 @@
         <v>43</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>745</v>
+        <v>1071</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>746</v>
+        <v>1072</v>
       </c>
       <c r="J15" s="3" t="s">
         <v>246</v>
@@ -43993,7 +44731,7 @@
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A16" s="163" t="s">
-        <v>786</v>
+        <v>1086</v>
       </c>
       <c r="B16" s="86" t="s">
         <v>73</v>
@@ -44011,13 +44749,13 @@
         <v>43</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>745</v>
+        <v>1071</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>746</v>
+        <v>1072</v>
       </c>
       <c r="J16" s="3" t="s">
         <v>246</v>
@@ -44040,7 +44778,7 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="163" t="s">
-        <v>789</v>
+        <v>1087</v>
       </c>
       <c r="B17" s="86" t="s">
         <v>75</v>
@@ -44058,13 +44796,13 @@
         <v>43</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>745</v>
+        <v>1071</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>746</v>
+        <v>1072</v>
       </c>
       <c r="J17" s="3" t="s">
         <v>246</v>
@@ -44087,7 +44825,7 @@
     </row>
     <row r="18" spans="1:15" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A18" s="163" t="s">
-        <v>792</v>
+        <v>1088</v>
       </c>
       <c r="B18" s="86" t="s">
         <v>793</v>
@@ -44105,13 +44843,13 @@
         <v>43</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>745</v>
+        <v>1071</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>746</v>
+        <v>1072</v>
       </c>
       <c r="J18" s="3" t="s">
         <v>246</v>
@@ -44134,7 +44872,7 @@
     </row>
     <row r="19" spans="1:15" ht="72" x14ac:dyDescent="0.3">
       <c r="A19" s="163" t="s">
-        <v>796</v>
+        <v>1089</v>
       </c>
       <c r="B19" s="86" t="s">
         <v>523</v>
@@ -44152,13 +44890,13 @@
         <v>43</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>745</v>
+        <v>1071</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>746</v>
+        <v>1072</v>
       </c>
       <c r="J19" s="3" t="s">
         <v>246</v>
@@ -44181,7 +44919,7 @@
     </row>
     <row r="20" spans="1:15" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A20" s="163" t="s">
-        <v>799</v>
+        <v>1090</v>
       </c>
       <c r="B20" s="86" t="s">
         <v>524</v>
@@ -44199,13 +44937,13 @@
         <v>43</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>745</v>
+        <v>1071</v>
       </c>
       <c r="H20" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>746</v>
+        <v>1072</v>
       </c>
       <c r="J20" s="3" t="s">
         <v>246</v>
@@ -44228,7 +44966,7 @@
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="163" t="s">
-        <v>802</v>
+        <v>1091</v>
       </c>
       <c r="B21" s="86" t="s">
         <v>82</v>
@@ -44246,13 +44984,13 @@
         <v>43</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>745</v>
+        <v>1071</v>
       </c>
       <c r="H21" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>746</v>
+        <v>1072</v>
       </c>
       <c r="J21" s="3" t="s">
         <v>246</v>
@@ -44275,7 +45013,7 @@
     </row>
     <row r="22" spans="1:15" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A22" s="163" t="s">
-        <v>805</v>
+        <v>1092</v>
       </c>
       <c r="B22" s="86" t="s">
         <v>526</v>
@@ -44293,13 +45031,13 @@
         <v>43</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>745</v>
+        <v>1071</v>
       </c>
       <c r="H22" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>746</v>
+        <v>1072</v>
       </c>
       <c r="J22" s="3" t="s">
         <v>246</v>
@@ -44322,7 +45060,7 @@
     </row>
     <row r="23" spans="1:15" ht="144" x14ac:dyDescent="0.3">
       <c r="A23" s="163" t="s">
-        <v>808</v>
+        <v>1093</v>
       </c>
       <c r="B23" s="86" t="s">
         <v>527</v>
@@ -44340,13 +45078,13 @@
         <v>43</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>745</v>
+        <v>1071</v>
       </c>
       <c r="H23" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>746</v>
+        <v>1072</v>
       </c>
       <c r="J23" s="3" t="s">
         <v>246</v>
@@ -44369,7 +45107,7 @@
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" s="163" t="s">
-        <v>811</v>
+        <v>1094</v>
       </c>
       <c r="B24" s="86" t="s">
         <v>84</v>
@@ -44387,13 +45125,13 @@
         <v>43</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>745</v>
+        <v>1071</v>
       </c>
       <c r="H24" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>746</v>
+        <v>1072</v>
       </c>
       <c r="J24" s="3" t="s">
         <v>246</v>
@@ -44416,7 +45154,7 @@
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" s="163" t="s">
-        <v>814</v>
+        <v>1095</v>
       </c>
       <c r="B25" s="86" t="s">
         <v>85</v>
@@ -44434,13 +45172,13 @@
         <v>43</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>745</v>
+        <v>1071</v>
       </c>
       <c r="H25" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>746</v>
+        <v>1072</v>
       </c>
       <c r="J25" s="3" t="s">
         <v>246</v>
@@ -44463,7 +45201,7 @@
     </row>
     <row r="26" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="163" t="s">
-        <v>817</v>
+        <v>1096</v>
       </c>
       <c r="B26" s="86" t="s">
         <v>88</v>
@@ -44481,13 +45219,13 @@
         <v>43</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>745</v>
+        <v>1071</v>
       </c>
       <c r="H26" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>746</v>
+        <v>1072</v>
       </c>
       <c r="J26" s="3" t="s">
         <v>246</v>
@@ -44510,7 +45248,7 @@
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" s="163" t="s">
-        <v>820</v>
+        <v>1097</v>
       </c>
       <c r="B27" s="86" t="s">
         <v>90</v>
@@ -44528,13 +45266,13 @@
         <v>43</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>745</v>
+        <v>1071</v>
       </c>
       <c r="H27" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>746</v>
+        <v>1072</v>
       </c>
       <c r="J27" s="3" t="s">
         <v>246</v>
@@ -44557,7 +45295,7 @@
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" s="163" t="s">
-        <v>823</v>
+        <v>1098</v>
       </c>
       <c r="B28" s="86" t="s">
         <v>91</v>
@@ -44575,13 +45313,13 @@
         <v>43</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>745</v>
+        <v>1071</v>
       </c>
       <c r="H28" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>746</v>
+        <v>1072</v>
       </c>
       <c r="J28" s="3" t="s">
         <v>246</v>
@@ -44604,7 +45342,7 @@
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" s="163" t="s">
-        <v>826</v>
+        <v>1099</v>
       </c>
       <c r="B29" s="86" t="s">
         <v>95</v>
@@ -44622,13 +45360,13 @@
         <v>43</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>745</v>
+        <v>1071</v>
       </c>
       <c r="H29" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>746</v>
+        <v>1072</v>
       </c>
       <c r="J29" s="3" t="s">
         <v>246</v>
@@ -44651,7 +45389,7 @@
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" s="163" t="s">
-        <v>829</v>
+        <v>1100</v>
       </c>
       <c r="B30" s="86" t="s">
         <v>98</v>
@@ -44669,13 +45407,13 @@
         <v>43</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>745</v>
+        <v>1071</v>
       </c>
       <c r="H30" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>746</v>
+        <v>1072</v>
       </c>
       <c r="J30" s="3" t="s">
         <v>246</v>
@@ -44698,7 +45436,7 @@
     </row>
     <row r="31" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="163" t="s">
-        <v>832</v>
+        <v>1101</v>
       </c>
       <c r="B31" s="86" t="s">
         <v>697</v>
@@ -44716,13 +45454,13 @@
         <v>43</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>745</v>
+        <v>1071</v>
       </c>
       <c r="H31" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>746</v>
+        <v>1072</v>
       </c>
       <c r="J31" s="3" t="s">
         <v>246</v>
@@ -44745,7 +45483,7 @@
     </row>
     <row r="32" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="163" t="s">
-        <v>837</v>
+        <v>1102</v>
       </c>
       <c r="B32" s="86" t="s">
         <v>704</v>
@@ -44763,13 +45501,13 @@
         <v>43</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>745</v>
+        <v>1071</v>
       </c>
       <c r="H32" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>746</v>
+        <v>1072</v>
       </c>
       <c r="J32" s="3" t="s">
         <v>246</v>
@@ -44792,7 +45530,7 @@
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" s="163" t="s">
-        <v>840</v>
+        <v>1103</v>
       </c>
       <c r="B33" s="86" t="s">
         <v>531</v>
@@ -44810,13 +45548,13 @@
         <v>43</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>745</v>
+        <v>1071</v>
       </c>
       <c r="H33" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>746</v>
+        <v>1072</v>
       </c>
       <c r="J33" s="3" t="s">
         <v>246</v>
@@ -44839,7 +45577,7 @@
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34" s="163" t="s">
-        <v>843</v>
+        <v>1104</v>
       </c>
       <c r="B34" s="86" t="s">
         <v>102</v>
@@ -44857,13 +45595,13 @@
         <v>43</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>745</v>
+        <v>1071</v>
       </c>
       <c r="H34" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>746</v>
+        <v>1072</v>
       </c>
       <c r="J34" s="3" t="s">
         <v>246</v>
@@ -44886,7 +45624,7 @@
     </row>
     <row r="35">
       <c r="A35" t="s" s="163">
-        <v>846</v>
+        <v>1105</v>
       </c>
       <c r="B35" t="s" s="86">
         <v>104</v>
@@ -44904,13 +45642,13 @@
         <v>43</v>
       </c>
       <c r="G35" t="s" s="3">
-        <v>745</v>
+        <v>1071</v>
       </c>
       <c r="H35" t="s" s="3">
         <v>337</v>
       </c>
       <c r="I35" t="s" s="3">
-        <v>746</v>
+        <v>1072</v>
       </c>
       <c r="J35" t="s" s="3">
         <v>246</v>
@@ -44933,7 +45671,7 @@
     </row>
     <row r="36">
       <c r="A36" t="s" s="163">
-        <v>849</v>
+        <v>1106</v>
       </c>
       <c r="B36" t="s" s="86">
         <v>106</v>
@@ -44951,13 +45689,13 @@
         <v>43</v>
       </c>
       <c r="G36" t="s" s="3">
-        <v>745</v>
+        <v>1071</v>
       </c>
       <c r="H36" t="s" s="3">
         <v>337</v>
       </c>
       <c r="I36" t="s" s="3">
-        <v>746</v>
+        <v>1072</v>
       </c>
       <c r="J36" t="s" s="3">
         <v>246</v>
@@ -44980,7 +45718,7 @@
     </row>
     <row r="37">
       <c r="A37" t="s" s="163">
-        <v>852</v>
+        <v>1107</v>
       </c>
       <c r="B37" t="s" s="86">
         <v>722</v>
@@ -44998,13 +45736,13 @@
         <v>43</v>
       </c>
       <c r="G37" t="s" s="3">
-        <v>745</v>
+        <v>1071</v>
       </c>
       <c r="H37" t="s" s="3">
         <v>337</v>
       </c>
       <c r="I37" t="s" s="3">
-        <v>746</v>
+        <v>1072</v>
       </c>
       <c r="J37" t="s" s="3">
         <v>246</v>
@@ -45027,7 +45765,7 @@
     </row>
     <row r="38">
       <c r="A38" t="s" s="163">
-        <v>856</v>
+        <v>1108</v>
       </c>
       <c r="B38" t="s" s="86">
         <v>728</v>
@@ -45045,13 +45783,13 @@
         <v>43</v>
       </c>
       <c r="G38" t="s" s="3">
-        <v>745</v>
+        <v>1071</v>
       </c>
       <c r="H38" t="s" s="3">
         <v>337</v>
       </c>
       <c r="I38" t="s" s="3">
-        <v>746</v>
+        <v>1072</v>
       </c>
       <c r="J38" t="s" s="3">
         <v>246</v>
@@ -45074,7 +45812,7 @@
     </row>
     <row r="39">
       <c r="A39" t="s" s="163">
-        <v>859</v>
+        <v>1109</v>
       </c>
       <c r="B39" t="s" s="86">
         <v>733</v>
@@ -45092,13 +45830,13 @@
         <v>43</v>
       </c>
       <c r="G39" t="s" s="3">
-        <v>745</v>
+        <v>1071</v>
       </c>
       <c r="H39" t="s" s="3">
         <v>337</v>
       </c>
       <c r="I39" t="s" s="3">
-        <v>746</v>
+        <v>1072</v>
       </c>
       <c r="J39" t="s" s="3">
         <v>246</v>
@@ -45121,7 +45859,7 @@
     </row>
     <row r="40">
       <c r="A40" t="s" s="163">
-        <v>862</v>
+        <v>1110</v>
       </c>
       <c r="B40" t="s" s="86">
         <v>738</v>
@@ -45139,13 +45877,13 @@
         <v>43</v>
       </c>
       <c r="G40" t="s" s="3">
-        <v>745</v>
+        <v>1071</v>
       </c>
       <c r="H40" t="s" s="3">
         <v>337</v>
       </c>
       <c r="I40" t="s" s="3">
-        <v>746</v>
+        <v>1072</v>
       </c>
       <c r="J40" t="s" s="3">
         <v>246</v>

</xml_diff>

<commit_message>
sinlge cat Automation enviroiment
</commit_message>
<xml_diff>
--- a/target/ExcelCalculatorForDistributor/Arshad New Calculator.xlsx
+++ b/target/ExcelCalculatorForDistributor/Arshad New Calculator.xlsx
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52283" uniqueCount="1111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63901" uniqueCount="1316">
   <si>
     <t>id</t>
   </si>
@@ -3499,6 +3499,621 @@
   </si>
   <si>
     <t>55744</t>
+  </si>
+  <si>
+    <t>55745</t>
+  </si>
+  <si>
+    <t>1706</t>
+  </si>
+  <si>
+    <t>TEST-ABC-0125-1-0127</t>
+  </si>
+  <si>
+    <t>55746</t>
+  </si>
+  <si>
+    <t>55747</t>
+  </si>
+  <si>
+    <t>55748</t>
+  </si>
+  <si>
+    <t>55749</t>
+  </si>
+  <si>
+    <t>55750</t>
+  </si>
+  <si>
+    <t>55751</t>
+  </si>
+  <si>
+    <t>55752</t>
+  </si>
+  <si>
+    <t>55753</t>
+  </si>
+  <si>
+    <t>55754</t>
+  </si>
+  <si>
+    <t>55755</t>
+  </si>
+  <si>
+    <t>55756</t>
+  </si>
+  <si>
+    <t>55757</t>
+  </si>
+  <si>
+    <t>55758</t>
+  </si>
+  <si>
+    <t>55759</t>
+  </si>
+  <si>
+    <t>55760</t>
+  </si>
+  <si>
+    <t>55761</t>
+  </si>
+  <si>
+    <t>55762</t>
+  </si>
+  <si>
+    <t>55763</t>
+  </si>
+  <si>
+    <t>55764</t>
+  </si>
+  <si>
+    <t>55765</t>
+  </si>
+  <si>
+    <t>55766</t>
+  </si>
+  <si>
+    <t>55767</t>
+  </si>
+  <si>
+    <t>55768</t>
+  </si>
+  <si>
+    <t>55769</t>
+  </si>
+  <si>
+    <t>55770</t>
+  </si>
+  <si>
+    <t>55771</t>
+  </si>
+  <si>
+    <t>55772</t>
+  </si>
+  <si>
+    <t>55773</t>
+  </si>
+  <si>
+    <t>55774</t>
+  </si>
+  <si>
+    <t>55775</t>
+  </si>
+  <si>
+    <t>55776</t>
+  </si>
+  <si>
+    <t>55777</t>
+  </si>
+  <si>
+    <t>55778</t>
+  </si>
+  <si>
+    <t>55779</t>
+  </si>
+  <si>
+    <t>55780</t>
+  </si>
+  <si>
+    <t>55781</t>
+  </si>
+  <si>
+    <t>55782</t>
+  </si>
+  <si>
+    <t>55783</t>
+  </si>
+  <si>
+    <t>55784</t>
+  </si>
+  <si>
+    <t>1707</t>
+  </si>
+  <si>
+    <t>TEST-ABC-0125-1-0128</t>
+  </si>
+  <si>
+    <t>55785</t>
+  </si>
+  <si>
+    <t>55786</t>
+  </si>
+  <si>
+    <t>55787</t>
+  </si>
+  <si>
+    <t>55788</t>
+  </si>
+  <si>
+    <t>55789</t>
+  </si>
+  <si>
+    <t>55790</t>
+  </si>
+  <si>
+    <t>55791</t>
+  </si>
+  <si>
+    <t>55792</t>
+  </si>
+  <si>
+    <t>55793</t>
+  </si>
+  <si>
+    <t>55794</t>
+  </si>
+  <si>
+    <t>55795</t>
+  </si>
+  <si>
+    <t>55796</t>
+  </si>
+  <si>
+    <t>55797</t>
+  </si>
+  <si>
+    <t>55798</t>
+  </si>
+  <si>
+    <t>55799</t>
+  </si>
+  <si>
+    <t>55800</t>
+  </si>
+  <si>
+    <t>55801</t>
+  </si>
+  <si>
+    <t>55802</t>
+  </si>
+  <si>
+    <t>55803</t>
+  </si>
+  <si>
+    <t>55804</t>
+  </si>
+  <si>
+    <t>55805</t>
+  </si>
+  <si>
+    <t>55806</t>
+  </si>
+  <si>
+    <t>55807</t>
+  </si>
+  <si>
+    <t>55808</t>
+  </si>
+  <si>
+    <t>55809</t>
+  </si>
+  <si>
+    <t>55810</t>
+  </si>
+  <si>
+    <t>55811</t>
+  </si>
+  <si>
+    <t>55812</t>
+  </si>
+  <si>
+    <t>55813</t>
+  </si>
+  <si>
+    <t>55814</t>
+  </si>
+  <si>
+    <t>55815</t>
+  </si>
+  <si>
+    <t>55816</t>
+  </si>
+  <si>
+    <t>55817</t>
+  </si>
+  <si>
+    <t>55818</t>
+  </si>
+  <si>
+    <t>55819</t>
+  </si>
+  <si>
+    <t>55820</t>
+  </si>
+  <si>
+    <t>55821</t>
+  </si>
+  <si>
+    <t>55822</t>
+  </si>
+  <si>
+    <t>56095</t>
+  </si>
+  <si>
+    <t>1715</t>
+  </si>
+  <si>
+    <t>TEST-ABC-0125-1-0136</t>
+  </si>
+  <si>
+    <t>56096</t>
+  </si>
+  <si>
+    <t>56097</t>
+  </si>
+  <si>
+    <t>56098</t>
+  </si>
+  <si>
+    <t>56099</t>
+  </si>
+  <si>
+    <t>56100</t>
+  </si>
+  <si>
+    <t>56101</t>
+  </si>
+  <si>
+    <t>56102</t>
+  </si>
+  <si>
+    <t>56103</t>
+  </si>
+  <si>
+    <t>56104</t>
+  </si>
+  <si>
+    <t>56105</t>
+  </si>
+  <si>
+    <t>56106</t>
+  </si>
+  <si>
+    <t>56107</t>
+  </si>
+  <si>
+    <t>56108</t>
+  </si>
+  <si>
+    <t>56109</t>
+  </si>
+  <si>
+    <t>56110</t>
+  </si>
+  <si>
+    <t>56111</t>
+  </si>
+  <si>
+    <t>56112</t>
+  </si>
+  <si>
+    <t>56113</t>
+  </si>
+  <si>
+    <t>56114</t>
+  </si>
+  <si>
+    <t>56115</t>
+  </si>
+  <si>
+    <t>56116</t>
+  </si>
+  <si>
+    <t>56117</t>
+  </si>
+  <si>
+    <t>56118</t>
+  </si>
+  <si>
+    <t>56119</t>
+  </si>
+  <si>
+    <t>56120</t>
+  </si>
+  <si>
+    <t>56121</t>
+  </si>
+  <si>
+    <t>56122</t>
+  </si>
+  <si>
+    <t>56123</t>
+  </si>
+  <si>
+    <t>56124</t>
+  </si>
+  <si>
+    <t>56125</t>
+  </si>
+  <si>
+    <t>56126</t>
+  </si>
+  <si>
+    <t>56127</t>
+  </si>
+  <si>
+    <t>56128</t>
+  </si>
+  <si>
+    <t>56129</t>
+  </si>
+  <si>
+    <t>56130</t>
+  </si>
+  <si>
+    <t>56131</t>
+  </si>
+  <si>
+    <t>56132</t>
+  </si>
+  <si>
+    <t>56133</t>
+  </si>
+  <si>
+    <t>56173</t>
+  </si>
+  <si>
+    <t>1717</t>
+  </si>
+  <si>
+    <t>TEST-ABC-0125-1-0138</t>
+  </si>
+  <si>
+    <t>56174</t>
+  </si>
+  <si>
+    <t>56175</t>
+  </si>
+  <si>
+    <t>56176</t>
+  </si>
+  <si>
+    <t>56177</t>
+  </si>
+  <si>
+    <t>56178</t>
+  </si>
+  <si>
+    <t>56179</t>
+  </si>
+  <si>
+    <t>56180</t>
+  </si>
+  <si>
+    <t>56181</t>
+  </si>
+  <si>
+    <t>56182</t>
+  </si>
+  <si>
+    <t>56183</t>
+  </si>
+  <si>
+    <t>56184</t>
+  </si>
+  <si>
+    <t>56185</t>
+  </si>
+  <si>
+    <t>56186</t>
+  </si>
+  <si>
+    <t>56187</t>
+  </si>
+  <si>
+    <t>56188</t>
+  </si>
+  <si>
+    <t>56189</t>
+  </si>
+  <si>
+    <t>56190</t>
+  </si>
+  <si>
+    <t>56191</t>
+  </si>
+  <si>
+    <t>56192</t>
+  </si>
+  <si>
+    <t>56193</t>
+  </si>
+  <si>
+    <t>56194</t>
+  </si>
+  <si>
+    <t>56195</t>
+  </si>
+  <si>
+    <t>56196</t>
+  </si>
+  <si>
+    <t>56197</t>
+  </si>
+  <si>
+    <t>56198</t>
+  </si>
+  <si>
+    <t>56199</t>
+  </si>
+  <si>
+    <t>56200</t>
+  </si>
+  <si>
+    <t>56201</t>
+  </si>
+  <si>
+    <t>56202</t>
+  </si>
+  <si>
+    <t>56203</t>
+  </si>
+  <si>
+    <t>56204</t>
+  </si>
+  <si>
+    <t>56205</t>
+  </si>
+  <si>
+    <t>56206</t>
+  </si>
+  <si>
+    <t>56207</t>
+  </si>
+  <si>
+    <t>56208</t>
+  </si>
+  <si>
+    <t>56209</t>
+  </si>
+  <si>
+    <t>56210</t>
+  </si>
+  <si>
+    <t>56211</t>
+  </si>
+  <si>
+    <t>56290</t>
+  </si>
+  <si>
+    <t>1720</t>
+  </si>
+  <si>
+    <t>TEST-ABC-0225-1-000001</t>
+  </si>
+  <si>
+    <t>56291</t>
+  </si>
+  <si>
+    <t>56292</t>
+  </si>
+  <si>
+    <t>56293</t>
+  </si>
+  <si>
+    <t>56294</t>
+  </si>
+  <si>
+    <t>56295</t>
+  </si>
+  <si>
+    <t>56296</t>
+  </si>
+  <si>
+    <t>56297</t>
+  </si>
+  <si>
+    <t>56298</t>
+  </si>
+  <si>
+    <t>56299</t>
+  </si>
+  <si>
+    <t>56300</t>
+  </si>
+  <si>
+    <t>56301</t>
+  </si>
+  <si>
+    <t>56302</t>
+  </si>
+  <si>
+    <t>56303</t>
+  </si>
+  <si>
+    <t>56304</t>
+  </si>
+  <si>
+    <t>56305</t>
+  </si>
+  <si>
+    <t>56306</t>
+  </si>
+  <si>
+    <t>56307</t>
+  </si>
+  <si>
+    <t>56308</t>
+  </si>
+  <si>
+    <t>56309</t>
+  </si>
+  <si>
+    <t>56310</t>
+  </si>
+  <si>
+    <t>56311</t>
+  </si>
+  <si>
+    <t>56312</t>
+  </si>
+  <si>
+    <t>56313</t>
+  </si>
+  <si>
+    <t>56314</t>
+  </si>
+  <si>
+    <t>56315</t>
+  </si>
+  <si>
+    <t>56316</t>
+  </si>
+  <si>
+    <t>56317</t>
+  </si>
+  <si>
+    <t>56318</t>
+  </si>
+  <si>
+    <t>56319</t>
+  </si>
+  <si>
+    <t>56320</t>
+  </si>
+  <si>
+    <t>56321</t>
+  </si>
+  <si>
+    <t>56322</t>
+  </si>
+  <si>
+    <t>56323</t>
+  </si>
+  <si>
+    <t>56324</t>
+  </si>
+  <si>
+    <t>56325</t>
+  </si>
+  <si>
+    <t>56326</t>
+  </si>
+  <si>
+    <t>56327</t>
+  </si>
+  <si>
+    <t>56328</t>
   </si>
 </sst>
 </file>
@@ -44073,7 +44688,7 @@
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" s="163" t="s">
-        <v>1070</v>
+        <v>1275</v>
       </c>
       <c r="B2" s="86" t="s">
         <v>42</v>
@@ -44091,13 +44706,13 @@
         <v>43</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>1071</v>
+        <v>1276</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>1072</v>
+        <v>1277</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>246</v>
@@ -44120,7 +44735,7 @@
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" s="163" t="s">
-        <v>1073</v>
+        <v>1278</v>
       </c>
       <c r="B3" s="86" t="s">
         <v>48</v>
@@ -44138,13 +44753,13 @@
         <v>43</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>1071</v>
+        <v>1276</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>1072</v>
+        <v>1277</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>246</v>
@@ -44167,7 +44782,7 @@
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A4" s="163" t="s">
-        <v>1074</v>
+        <v>1279</v>
       </c>
       <c r="B4" s="86" t="s">
         <v>50</v>
@@ -44185,13 +44800,13 @@
         <v>43</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>1071</v>
+        <v>1276</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>1072</v>
+        <v>1277</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>246</v>
@@ -44214,7 +44829,7 @@
     </row>
     <row r="5" spans="1:25" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="163" t="s">
-        <v>1075</v>
+        <v>1280</v>
       </c>
       <c r="B5" s="86" t="s">
         <v>52</v>
@@ -44232,13 +44847,13 @@
         <v>43</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>1071</v>
+        <v>1276</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>1072</v>
+        <v>1277</v>
       </c>
       <c r="J5" s="3" t="s">
         <v>246</v>
@@ -44261,7 +44876,7 @@
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A6" s="163" t="s">
-        <v>1076</v>
+        <v>1281</v>
       </c>
       <c r="B6" s="86" t="s">
         <v>53</v>
@@ -44279,13 +44894,13 @@
         <v>43</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>1071</v>
+        <v>1276</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>1072</v>
+        <v>1277</v>
       </c>
       <c r="J6" s="3" t="s">
         <v>246</v>
@@ -44308,7 +44923,7 @@
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A7" s="163" t="s">
-        <v>1077</v>
+        <v>1282</v>
       </c>
       <c r="B7" s="86" t="s">
         <v>54</v>
@@ -44326,13 +44941,13 @@
         <v>43</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>1071</v>
+        <v>1276</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>1072</v>
+        <v>1277</v>
       </c>
       <c r="J7" s="3" t="s">
         <v>246</v>
@@ -44355,7 +44970,7 @@
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A8" s="163" t="s">
-        <v>1078</v>
+        <v>1283</v>
       </c>
       <c r="B8" s="86" t="s">
         <v>57</v>
@@ -44373,13 +44988,13 @@
         <v>43</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>1071</v>
+        <v>1276</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>1072</v>
+        <v>1277</v>
       </c>
       <c r="J8" s="3" t="s">
         <v>246</v>
@@ -44402,7 +45017,7 @@
     </row>
     <row r="9" spans="1:25" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="163" t="s">
-        <v>1079</v>
+        <v>1284</v>
       </c>
       <c r="B9" s="86" t="s">
         <v>59</v>
@@ -44420,13 +45035,13 @@
         <v>43</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>1071</v>
+        <v>1276</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>1072</v>
+        <v>1277</v>
       </c>
       <c r="J9" s="3" t="s">
         <v>246</v>
@@ -44449,7 +45064,7 @@
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A10" s="163" t="s">
-        <v>1080</v>
+        <v>1285</v>
       </c>
       <c r="B10" s="86" t="s">
         <v>61</v>
@@ -44467,13 +45082,13 @@
         <v>43</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>1071</v>
+        <v>1276</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>1072</v>
+        <v>1277</v>
       </c>
       <c r="J10" s="3" t="s">
         <v>246</v>
@@ -44496,7 +45111,7 @@
     </row>
     <row r="11" spans="1:25" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" s="163" t="s">
-        <v>1081</v>
+        <v>1286</v>
       </c>
       <c r="B11" s="86" t="s">
         <v>62</v>
@@ -44514,13 +45129,13 @@
         <v>43</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>1071</v>
+        <v>1276</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>1072</v>
+        <v>1277</v>
       </c>
       <c r="J11" s="3" t="s">
         <v>246</v>
@@ -44543,7 +45158,7 @@
     </row>
     <row r="12" spans="1:25" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="163" t="s">
-        <v>1082</v>
+        <v>1287</v>
       </c>
       <c r="B12" s="86" t="s">
         <v>63</v>
@@ -44561,13 +45176,13 @@
         <v>43</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>1071</v>
+        <v>1276</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>1072</v>
+        <v>1277</v>
       </c>
       <c r="J12" s="3" t="s">
         <v>246</v>
@@ -44590,7 +45205,7 @@
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A13" s="163" t="s">
-        <v>1083</v>
+        <v>1288</v>
       </c>
       <c r="B13" s="86" t="s">
         <v>64</v>
@@ -44608,13 +45223,13 @@
         <v>43</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>1071</v>
+        <v>1276</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>1072</v>
+        <v>1277</v>
       </c>
       <c r="J13" s="3" t="s">
         <v>246</v>
@@ -44637,7 +45252,7 @@
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A14" s="163" t="s">
-        <v>1084</v>
+        <v>1289</v>
       </c>
       <c r="B14" s="86" t="s">
         <v>68</v>
@@ -44655,13 +45270,13 @@
         <v>43</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>1071</v>
+        <v>1276</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>1072</v>
+        <v>1277</v>
       </c>
       <c r="J14" s="3" t="s">
         <v>246</v>
@@ -44684,7 +45299,7 @@
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A15" s="163" t="s">
-        <v>1085</v>
+        <v>1290</v>
       </c>
       <c r="B15" s="86" t="s">
         <v>71</v>
@@ -44702,13 +45317,13 @@
         <v>43</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>1071</v>
+        <v>1276</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>1072</v>
+        <v>1277</v>
       </c>
       <c r="J15" s="3" t="s">
         <v>246</v>
@@ -44731,7 +45346,7 @@
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A16" s="163" t="s">
-        <v>1086</v>
+        <v>1291</v>
       </c>
       <c r="B16" s="86" t="s">
         <v>73</v>
@@ -44749,13 +45364,13 @@
         <v>43</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>1071</v>
+        <v>1276</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>1072</v>
+        <v>1277</v>
       </c>
       <c r="J16" s="3" t="s">
         <v>246</v>
@@ -44778,7 +45393,7 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="163" t="s">
-        <v>1087</v>
+        <v>1292</v>
       </c>
       <c r="B17" s="86" t="s">
         <v>75</v>
@@ -44796,13 +45411,13 @@
         <v>43</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>1071</v>
+        <v>1276</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>1072</v>
+        <v>1277</v>
       </c>
       <c r="J17" s="3" t="s">
         <v>246</v>
@@ -44825,7 +45440,7 @@
     </row>
     <row r="18" spans="1:15" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A18" s="163" t="s">
-        <v>1088</v>
+        <v>1293</v>
       </c>
       <c r="B18" s="86" t="s">
         <v>793</v>
@@ -44843,13 +45458,13 @@
         <v>43</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>1071</v>
+        <v>1276</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>1072</v>
+        <v>1277</v>
       </c>
       <c r="J18" s="3" t="s">
         <v>246</v>
@@ -44872,7 +45487,7 @@
     </row>
     <row r="19" spans="1:15" ht="72" x14ac:dyDescent="0.3">
       <c r="A19" s="163" t="s">
-        <v>1089</v>
+        <v>1294</v>
       </c>
       <c r="B19" s="86" t="s">
         <v>523</v>
@@ -44890,13 +45505,13 @@
         <v>43</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>1071</v>
+        <v>1276</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>1072</v>
+        <v>1277</v>
       </c>
       <c r="J19" s="3" t="s">
         <v>246</v>
@@ -44919,7 +45534,7 @@
     </row>
     <row r="20" spans="1:15" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A20" s="163" t="s">
-        <v>1090</v>
+        <v>1295</v>
       </c>
       <c r="B20" s="86" t="s">
         <v>524</v>
@@ -44937,13 +45552,13 @@
         <v>43</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>1071</v>
+        <v>1276</v>
       </c>
       <c r="H20" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>1072</v>
+        <v>1277</v>
       </c>
       <c r="J20" s="3" t="s">
         <v>246</v>
@@ -44966,7 +45581,7 @@
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="163" t="s">
-        <v>1091</v>
+        <v>1296</v>
       </c>
       <c r="B21" s="86" t="s">
         <v>82</v>
@@ -44984,13 +45599,13 @@
         <v>43</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>1071</v>
+        <v>1276</v>
       </c>
       <c r="H21" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>1072</v>
+        <v>1277</v>
       </c>
       <c r="J21" s="3" t="s">
         <v>246</v>
@@ -45013,7 +45628,7 @@
     </row>
     <row r="22" spans="1:15" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A22" s="163" t="s">
-        <v>1092</v>
+        <v>1297</v>
       </c>
       <c r="B22" s="86" t="s">
         <v>526</v>
@@ -45031,13 +45646,13 @@
         <v>43</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>1071</v>
+        <v>1276</v>
       </c>
       <c r="H22" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>1072</v>
+        <v>1277</v>
       </c>
       <c r="J22" s="3" t="s">
         <v>246</v>
@@ -45060,7 +45675,7 @@
     </row>
     <row r="23" spans="1:15" ht="144" x14ac:dyDescent="0.3">
       <c r="A23" s="163" t="s">
-        <v>1093</v>
+        <v>1298</v>
       </c>
       <c r="B23" s="86" t="s">
         <v>527</v>
@@ -45078,13 +45693,13 @@
         <v>43</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>1071</v>
+        <v>1276</v>
       </c>
       <c r="H23" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>1072</v>
+        <v>1277</v>
       </c>
       <c r="J23" s="3" t="s">
         <v>246</v>
@@ -45107,7 +45722,7 @@
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" s="163" t="s">
-        <v>1094</v>
+        <v>1299</v>
       </c>
       <c r="B24" s="86" t="s">
         <v>84</v>
@@ -45125,13 +45740,13 @@
         <v>43</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>1071</v>
+        <v>1276</v>
       </c>
       <c r="H24" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>1072</v>
+        <v>1277</v>
       </c>
       <c r="J24" s="3" t="s">
         <v>246</v>
@@ -45154,7 +45769,7 @@
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" s="163" t="s">
-        <v>1095</v>
+        <v>1300</v>
       </c>
       <c r="B25" s="86" t="s">
         <v>85</v>
@@ -45172,13 +45787,13 @@
         <v>43</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>1071</v>
+        <v>1276</v>
       </c>
       <c r="H25" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>1072</v>
+        <v>1277</v>
       </c>
       <c r="J25" s="3" t="s">
         <v>246</v>
@@ -45201,7 +45816,7 @@
     </row>
     <row r="26" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="163" t="s">
-        <v>1096</v>
+        <v>1301</v>
       </c>
       <c r="B26" s="86" t="s">
         <v>88</v>
@@ -45219,13 +45834,13 @@
         <v>43</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>1071</v>
+        <v>1276</v>
       </c>
       <c r="H26" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>1072</v>
+        <v>1277</v>
       </c>
       <c r="J26" s="3" t="s">
         <v>246</v>
@@ -45248,7 +45863,7 @@
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" s="163" t="s">
-        <v>1097</v>
+        <v>1302</v>
       </c>
       <c r="B27" s="86" t="s">
         <v>90</v>
@@ -45266,13 +45881,13 @@
         <v>43</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>1071</v>
+        <v>1276</v>
       </c>
       <c r="H27" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>1072</v>
+        <v>1277</v>
       </c>
       <c r="J27" s="3" t="s">
         <v>246</v>
@@ -45295,7 +45910,7 @@
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" s="163" t="s">
-        <v>1098</v>
+        <v>1303</v>
       </c>
       <c r="B28" s="86" t="s">
         <v>91</v>
@@ -45313,13 +45928,13 @@
         <v>43</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>1071</v>
+        <v>1276</v>
       </c>
       <c r="H28" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>1072</v>
+        <v>1277</v>
       </c>
       <c r="J28" s="3" t="s">
         <v>246</v>
@@ -45342,7 +45957,7 @@
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" s="163" t="s">
-        <v>1099</v>
+        <v>1304</v>
       </c>
       <c r="B29" s="86" t="s">
         <v>95</v>
@@ -45360,13 +45975,13 @@
         <v>43</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>1071</v>
+        <v>1276</v>
       </c>
       <c r="H29" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>1072</v>
+        <v>1277</v>
       </c>
       <c r="J29" s="3" t="s">
         <v>246</v>
@@ -45389,7 +46004,7 @@
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" s="163" t="s">
-        <v>1100</v>
+        <v>1305</v>
       </c>
       <c r="B30" s="86" t="s">
         <v>98</v>
@@ -45407,13 +46022,13 @@
         <v>43</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>1071</v>
+        <v>1276</v>
       </c>
       <c r="H30" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>1072</v>
+        <v>1277</v>
       </c>
       <c r="J30" s="3" t="s">
         <v>246</v>
@@ -45436,7 +46051,7 @@
     </row>
     <row r="31" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="163" t="s">
-        <v>1101</v>
+        <v>1306</v>
       </c>
       <c r="B31" s="86" t="s">
         <v>697</v>
@@ -45454,13 +46069,13 @@
         <v>43</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>1071</v>
+        <v>1276</v>
       </c>
       <c r="H31" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>1072</v>
+        <v>1277</v>
       </c>
       <c r="J31" s="3" t="s">
         <v>246</v>
@@ -45483,7 +46098,7 @@
     </row>
     <row r="32" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="163" t="s">
-        <v>1102</v>
+        <v>1307</v>
       </c>
       <c r="B32" s="86" t="s">
         <v>704</v>
@@ -45501,13 +46116,13 @@
         <v>43</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>1071</v>
+        <v>1276</v>
       </c>
       <c r="H32" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>1072</v>
+        <v>1277</v>
       </c>
       <c r="J32" s="3" t="s">
         <v>246</v>
@@ -45530,7 +46145,7 @@
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" s="163" t="s">
-        <v>1103</v>
+        <v>1308</v>
       </c>
       <c r="B33" s="86" t="s">
         <v>531</v>
@@ -45548,13 +46163,13 @@
         <v>43</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>1071</v>
+        <v>1276</v>
       </c>
       <c r="H33" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>1072</v>
+        <v>1277</v>
       </c>
       <c r="J33" s="3" t="s">
         <v>246</v>
@@ -45577,7 +46192,7 @@
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34" s="163" t="s">
-        <v>1104</v>
+        <v>1309</v>
       </c>
       <c r="B34" s="86" t="s">
         <v>102</v>
@@ -45595,13 +46210,13 @@
         <v>43</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>1071</v>
+        <v>1276</v>
       </c>
       <c r="H34" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>1072</v>
+        <v>1277</v>
       </c>
       <c r="J34" s="3" t="s">
         <v>246</v>
@@ -45624,7 +46239,7 @@
     </row>
     <row r="35">
       <c r="A35" t="s" s="163">
-        <v>1105</v>
+        <v>1310</v>
       </c>
       <c r="B35" t="s" s="86">
         <v>104</v>
@@ -45642,13 +46257,13 @@
         <v>43</v>
       </c>
       <c r="G35" t="s" s="3">
-        <v>1071</v>
+        <v>1276</v>
       </c>
       <c r="H35" t="s" s="3">
         <v>337</v>
       </c>
       <c r="I35" t="s" s="3">
-        <v>1072</v>
+        <v>1277</v>
       </c>
       <c r="J35" t="s" s="3">
         <v>246</v>
@@ -45671,7 +46286,7 @@
     </row>
     <row r="36">
       <c r="A36" t="s" s="163">
-        <v>1106</v>
+        <v>1311</v>
       </c>
       <c r="B36" t="s" s="86">
         <v>106</v>
@@ -45689,13 +46304,13 @@
         <v>43</v>
       </c>
       <c r="G36" t="s" s="3">
-        <v>1071</v>
+        <v>1276</v>
       </c>
       <c r="H36" t="s" s="3">
         <v>337</v>
       </c>
       <c r="I36" t="s" s="3">
-        <v>1072</v>
+        <v>1277</v>
       </c>
       <c r="J36" t="s" s="3">
         <v>246</v>
@@ -45718,7 +46333,7 @@
     </row>
     <row r="37">
       <c r="A37" t="s" s="163">
-        <v>1107</v>
+        <v>1312</v>
       </c>
       <c r="B37" t="s" s="86">
         <v>722</v>
@@ -45736,13 +46351,13 @@
         <v>43</v>
       </c>
       <c r="G37" t="s" s="3">
-        <v>1071</v>
+        <v>1276</v>
       </c>
       <c r="H37" t="s" s="3">
         <v>337</v>
       </c>
       <c r="I37" t="s" s="3">
-        <v>1072</v>
+        <v>1277</v>
       </c>
       <c r="J37" t="s" s="3">
         <v>246</v>
@@ -45765,7 +46380,7 @@
     </row>
     <row r="38">
       <c r="A38" t="s" s="163">
-        <v>1108</v>
+        <v>1313</v>
       </c>
       <c r="B38" t="s" s="86">
         <v>728</v>
@@ -45783,13 +46398,13 @@
         <v>43</v>
       </c>
       <c r="G38" t="s" s="3">
-        <v>1071</v>
+        <v>1276</v>
       </c>
       <c r="H38" t="s" s="3">
         <v>337</v>
       </c>
       <c r="I38" t="s" s="3">
-        <v>1072</v>
+        <v>1277</v>
       </c>
       <c r="J38" t="s" s="3">
         <v>246</v>
@@ -45812,7 +46427,7 @@
     </row>
     <row r="39">
       <c r="A39" t="s" s="163">
-        <v>1109</v>
+        <v>1314</v>
       </c>
       <c r="B39" t="s" s="86">
         <v>733</v>
@@ -45830,13 +46445,13 @@
         <v>43</v>
       </c>
       <c r="G39" t="s" s="3">
-        <v>1071</v>
+        <v>1276</v>
       </c>
       <c r="H39" t="s" s="3">
         <v>337</v>
       </c>
       <c r="I39" t="s" s="3">
-        <v>1072</v>
+        <v>1277</v>
       </c>
       <c r="J39" t="s" s="3">
         <v>246</v>
@@ -45859,7 +46474,7 @@
     </row>
     <row r="40">
       <c r="A40" t="s" s="163">
-        <v>1110</v>
+        <v>1315</v>
       </c>
       <c r="B40" t="s" s="86">
         <v>738</v>
@@ -45877,13 +46492,13 @@
         <v>43</v>
       </c>
       <c r="G40" t="s" s="3">
-        <v>1071</v>
+        <v>1276</v>
       </c>
       <c r="H40" t="s" s="3">
         <v>337</v>
       </c>
       <c r="I40" t="s" s="3">
-        <v>1072</v>
+        <v>1277</v>
       </c>
       <c r="J40" t="s" s="3">
         <v>246</v>

</xml_diff>